<commit_message>
Addition of new sizes.
</commit_message>
<xml_diff>
--- a/windisch/data/Input data.xlsx
+++ b/windisch/data/Input data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/windisch/windisch/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhuber\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3844C490-07BB-1B4E-9780-6ED29D64154B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B8B361-E618-4EC8-B967-3125460ABD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28420" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$2:$Y$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$2:$Y$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="79">
   <si>
     <t>parameter</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>power</t>
+  </si>
+  <si>
+    <t>10000kW</t>
+  </si>
+  <si>
+    <t>15000kW</t>
+  </si>
+  <si>
+    <t>3400kW</t>
   </si>
 </sst>
 </file>
@@ -368,9 +377,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -408,9 +417,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -443,26 +452,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -495,26 +487,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -688,42 +663,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB43"/>
+  <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="26.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="8.83203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="8.77734375" style="1" customWidth="1"/>
     <col min="23" max="23" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="29" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -809,7 +785,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -875,7 +851,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -929,7 +905,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -983,7 +959,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1037,7 +1013,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1091,7 +1067,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1099,7 +1075,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>75</v>
@@ -1117,319 +1093,211 @@
         <v>10</v>
       </c>
       <c r="K7" s="1">
-        <v>8000</v>
+        <v>3400</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="1">
-        <v>8000</v>
+        <v>3400</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="1">
-        <v>8000</v>
+        <v>3400</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="1">
-        <v>8000</v>
+        <v>3400</v>
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
       <c r="W7" s="1">
-        <v>8000</v>
+        <v>3400</v>
       </c>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
       <c r="Z7" s="1">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="1">
         <v>8000</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="1">
+        <v>8000</v>
+      </c>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="1">
+        <v>8000</v>
+      </c>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="1">
+        <v>8000</v>
+      </c>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="1">
+        <v>8000</v>
+      </c>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="1">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="1">
+        <v>15000</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="1">
+        <v>15000</v>
+      </c>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="1">
+        <v>15000</v>
+      </c>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="1">
+        <v>15000</v>
+      </c>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="1">
+        <v>15000</v>
+      </c>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="1">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" s="1">
-        <v>30</v>
-      </c>
-      <c r="L8" s="1">
-        <v>25</v>
-      </c>
-      <c r="M8" s="1">
-        <v>35</v>
-      </c>
-      <c r="N8" s="1">
-        <v>30</v>
-      </c>
-      <c r="O8" s="1">
-        <v>25</v>
-      </c>
-      <c r="P8" s="1">
-        <v>35</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>30</v>
-      </c>
-      <c r="R8" s="1">
-        <v>25</v>
-      </c>
-      <c r="S8" s="1">
-        <v>35</v>
-      </c>
-      <c r="T8" s="1">
-        <v>30</v>
-      </c>
-      <c r="U8" s="1">
-        <v>25</v>
-      </c>
-      <c r="V8" s="1">
-        <v>35</v>
-      </c>
-      <c r="W8" s="1">
-        <v>30</v>
-      </c>
-      <c r="X8" s="1">
-        <v>25</v>
-      </c>
-      <c r="Y8" s="1">
-        <v>35</v>
-      </c>
-      <c r="Z8" s="1">
-        <v>30</v>
-      </c>
-      <c r="AA8" s="1">
-        <v>25</v>
-      </c>
-      <c r="AB8" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="1">
-        <v>600</v>
-      </c>
-      <c r="L9" s="1">
-        <f>K9*0.8</f>
-        <v>480</v>
-      </c>
-      <c r="M9" s="1">
-        <f>K9*1.2</f>
-        <v>720</v>
-      </c>
-      <c r="N9" s="1">
-        <v>600</v>
-      </c>
-      <c r="O9" s="1">
-        <f>N9*0.8</f>
-        <v>480</v>
-      </c>
-      <c r="P9" s="1">
-        <f>N9*1.2</f>
-        <v>720</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>600</v>
-      </c>
-      <c r="R9" s="1">
-        <f>Q9*0.8</f>
-        <v>480</v>
-      </c>
-      <c r="S9" s="1">
-        <f>Q9*1.2</f>
-        <v>720</v>
-      </c>
-      <c r="T9" s="1">
-        <v>600</v>
-      </c>
-      <c r="U9" s="1">
-        <f>T9*0.8</f>
-        <v>480</v>
-      </c>
-      <c r="V9" s="1">
-        <f>T9*1.2</f>
-        <v>720</v>
-      </c>
-      <c r="W9" s="1">
-        <v>600</v>
-      </c>
-      <c r="X9" s="1">
-        <f>W9*0.8</f>
-        <v>480</v>
-      </c>
-      <c r="Y9" s="1">
-        <f>W9*1.2</f>
-        <v>720</v>
-      </c>
-      <c r="Z9" s="1">
-        <v>600</v>
-      </c>
-      <c r="AA9" s="1">
-        <f>Z9*0.8</f>
-        <v>480</v>
-      </c>
-      <c r="AB9" s="1">
-        <f>Z9*1.2</f>
-        <v>720</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K10" s="1">
-        <v>1025</v>
-      </c>
-      <c r="L10" s="1">
-        <f>K10*0.8</f>
-        <v>820</v>
-      </c>
-      <c r="M10" s="1">
-        <f>K10*1.2</f>
-        <v>1230</v>
-      </c>
-      <c r="N10" s="1">
-        <v>1025</v>
-      </c>
-      <c r="O10" s="1">
-        <f>N10*0.8</f>
-        <v>820</v>
-      </c>
-      <c r="P10" s="1">
-        <f>N10*1.2</f>
-        <v>1230</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>1025</v>
-      </c>
-      <c r="R10" s="1">
-        <f>Q10*0.8</f>
-        <v>820</v>
-      </c>
-      <c r="S10" s="1">
-        <f>Q10*1.2</f>
-        <v>1230</v>
-      </c>
-      <c r="T10" s="1">
-        <v>1025</v>
-      </c>
-      <c r="U10" s="1">
-        <f>T10*0.8</f>
-        <v>820</v>
-      </c>
-      <c r="V10" s="1">
-        <f>T10*1.2</f>
-        <v>1230</v>
-      </c>
-      <c r="W10" s="1">
-        <v>1025</v>
-      </c>
-      <c r="X10" s="1">
-        <f>W10*0.8</f>
-        <v>820</v>
-      </c>
-      <c r="Y10" s="1">
-        <f>W10*1.2</f>
-        <v>1230</v>
-      </c>
-      <c r="Z10" s="1">
-        <v>1025</v>
-      </c>
-      <c r="AA10" s="1">
-        <f>Z10*0.8</f>
-        <v>820</v>
-      </c>
-      <c r="AB10" s="1">
-        <f>Z10*1.2</f>
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>23</v>
@@ -1437,82 +1305,67 @@
       <c r="G11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="J11" s="1" t="s">
         <v>56</v>
       </c>
       <c r="K11" s="1">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="L11" s="1">
-        <f>K11*0.8</f>
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="M11" s="1">
-        <f>K11*1.2</f>
-        <v>720</v>
+        <v>35</v>
       </c>
       <c r="N11" s="1">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="O11" s="1">
-        <f>N11*0.8</f>
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="P11" s="1">
-        <f>N11*1.2</f>
-        <v>720</v>
+        <v>35</v>
       </c>
       <c r="Q11" s="1">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="R11" s="1">
-        <f>Q11*0.8</f>
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="S11" s="1">
-        <f>Q11*1.2</f>
-        <v>720</v>
+        <v>35</v>
       </c>
       <c r="T11" s="1">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="U11" s="1">
-        <f>T11*0.8</f>
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="V11" s="1">
-        <f>T11*1.2</f>
-        <v>720</v>
+        <v>35</v>
       </c>
       <c r="W11" s="1">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="X11" s="1">
-        <f>W11*0.8</f>
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="Y11" s="1">
-        <f>W11*1.2</f>
-        <v>720</v>
+        <v>35</v>
       </c>
       <c r="Z11" s="1">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="AA11" s="1">
-        <f>Z11*0.8</f>
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="AB11" s="1">
-        <f>Z11*1.2</f>
-        <v>720</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>19</v>
@@ -1521,7 +1374,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>9</v>
@@ -1539,270 +1392,364 @@
         <v>56</v>
       </c>
       <c r="K12" s="1">
+        <v>600</v>
+      </c>
+      <c r="L12" s="1">
+        <f>K12*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="M12" s="1">
+        <f>K12*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="N12" s="1">
+        <v>600</v>
+      </c>
+      <c r="O12" s="1">
+        <f>N12*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="P12" s="1">
+        <f>N12*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>600</v>
+      </c>
+      <c r="R12" s="1">
+        <f>Q12*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="S12" s="1">
+        <f>Q12*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="T12" s="1">
+        <v>600</v>
+      </c>
+      <c r="U12" s="1">
+        <f>T12*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="V12" s="1">
+        <f>T12*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="W12" s="1">
+        <v>600</v>
+      </c>
+      <c r="X12" s="1">
+        <f>W12*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="Y12" s="1">
+        <f>W12*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>600</v>
+      </c>
+      <c r="AA12" s="1">
+        <f>Z12*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="AB12" s="1">
+        <f>Z12*1.2</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1025</v>
+      </c>
+      <c r="L13" s="1">
+        <f>K13*0.8</f>
+        <v>820</v>
+      </c>
+      <c r="M13" s="1">
+        <f>K13*1.2</f>
+        <v>1230</v>
+      </c>
+      <c r="N13" s="1">
+        <v>1025</v>
+      </c>
+      <c r="O13" s="1">
+        <f>N13*0.8</f>
+        <v>820</v>
+      </c>
+      <c r="P13" s="1">
+        <f>N13*1.2</f>
+        <v>1230</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>1025</v>
+      </c>
+      <c r="R13" s="1">
+        <f>Q13*0.8</f>
+        <v>820</v>
+      </c>
+      <c r="S13" s="1">
+        <f>Q13*1.2</f>
+        <v>1230</v>
+      </c>
+      <c r="T13" s="1">
+        <v>1025</v>
+      </c>
+      <c r="U13" s="1">
+        <f>T13*0.8</f>
+        <v>820</v>
+      </c>
+      <c r="V13" s="1">
+        <f>T13*1.2</f>
+        <v>1230</v>
+      </c>
+      <c r="W13" s="1">
+        <v>1025</v>
+      </c>
+      <c r="X13" s="1">
+        <f>W13*0.8</f>
+        <v>820</v>
+      </c>
+      <c r="Y13" s="1">
+        <f>W13*1.2</f>
+        <v>1230</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>1025</v>
+      </c>
+      <c r="AA13" s="1">
+        <f>Z13*0.8</f>
+        <v>820</v>
+      </c>
+      <c r="AB13" s="1">
+        <f>Z13*1.2</f>
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="1">
+        <v>600</v>
+      </c>
+      <c r="L14" s="1">
+        <f>K14*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="M14" s="1">
+        <f>K14*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="N14" s="1">
+        <v>600</v>
+      </c>
+      <c r="O14" s="1">
+        <f>N14*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="P14" s="1">
+        <f>N14*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>600</v>
+      </c>
+      <c r="R14" s="1">
+        <f>Q14*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="S14" s="1">
+        <f>Q14*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="T14" s="1">
+        <v>600</v>
+      </c>
+      <c r="U14" s="1">
+        <f>T14*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="V14" s="1">
+        <f>T14*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="W14" s="1">
+        <v>600</v>
+      </c>
+      <c r="X14" s="1">
+        <f>W14*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="Y14" s="1">
+        <f>W14*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>600</v>
+      </c>
+      <c r="AA14" s="1">
+        <f>Z14*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="AB14" s="1">
+        <f>Z14*1.2</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="1">
         <f>1100+8050</f>
         <v>9150</v>
       </c>
-      <c r="L12" s="1">
-        <f>K12*0.8</f>
+      <c r="L15" s="1">
+        <f>K15*0.8</f>
         <v>7320</v>
       </c>
-      <c r="M12" s="1">
-        <f>K12*1.2</f>
+      <c r="M15" s="1">
+        <f>K15*1.2</f>
         <v>10980</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N15" s="1">
         <f>1100+8050</f>
         <v>9150</v>
       </c>
-      <c r="O12" s="1">
-        <f>N12*0.8</f>
+      <c r="O15" s="1">
+        <f>N15*0.8</f>
         <v>7320</v>
       </c>
-      <c r="P12" s="1">
-        <f>N12*1.2</f>
+      <c r="P15" s="1">
+        <f>N15*1.2</f>
         <v>10980</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="Q15" s="1">
         <f>1100+8050</f>
         <v>9150</v>
       </c>
-      <c r="R12" s="1">
-        <f>Q12*0.8</f>
+      <c r="R15" s="1">
+        <f>Q15*0.8</f>
         <v>7320</v>
       </c>
-      <c r="S12" s="1">
-        <f>Q12*1.2</f>
+      <c r="S15" s="1">
+        <f>Q15*1.2</f>
         <v>10980</v>
       </c>
-      <c r="T12" s="1">
+      <c r="T15" s="1">
         <f>1100+8050</f>
         <v>9150</v>
       </c>
-      <c r="U12" s="1">
-        <f>T12*0.8</f>
+      <c r="U15" s="1">
+        <f>T15*0.8</f>
         <v>7320</v>
       </c>
-      <c r="V12" s="1">
-        <f>T12*1.2</f>
+      <c r="V15" s="1">
+        <f>T15*1.2</f>
         <v>10980</v>
       </c>
-      <c r="W12" s="1">
+      <c r="W15" s="1">
         <f>1100+8050</f>
         <v>9150</v>
       </c>
-      <c r="X12" s="1">
-        <f>W12*0.8</f>
+      <c r="X15" s="1">
+        <f>W15*0.8</f>
         <v>7320</v>
       </c>
-      <c r="Y12" s="1">
-        <f>W12*1.2</f>
+      <c r="Y15" s="1">
+        <f>W15*1.2</f>
         <v>10980</v>
       </c>
-      <c r="Z12" s="1">
+      <c r="Z15" s="1">
         <f>1100+8050</f>
         <v>9150</v>
       </c>
-      <c r="AA12" s="1">
-        <f>Z12*0.8</f>
+      <c r="AA15" s="1">
+        <f>Z15*0.8</f>
         <v>7320</v>
       </c>
-      <c r="AB12" s="1">
-        <f>Z12*1.2</f>
+      <c r="AB15" s="1">
+        <f>Z15*1.2</f>
         <v>10980</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K13" s="1">
-        <v>50</v>
-      </c>
-      <c r="L13" s="1">
-        <f t="shared" ref="L13:L30" si="0">K13*0.8</f>
-        <v>40</v>
-      </c>
-      <c r="M13" s="1">
-        <f t="shared" ref="M13" si="1">K13*1.2</f>
-        <v>60</v>
-      </c>
-      <c r="N13" s="1">
-        <v>50</v>
-      </c>
-      <c r="O13" s="1">
-        <f t="shared" ref="O13:O30" si="2">N13*0.8</f>
-        <v>40</v>
-      </c>
-      <c r="P13" s="1">
-        <f t="shared" ref="P13" si="3">N13*1.2</f>
-        <v>60</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>50</v>
-      </c>
-      <c r="R13" s="1">
-        <f t="shared" ref="R13:R30" si="4">Q13*0.8</f>
-        <v>40</v>
-      </c>
-      <c r="S13" s="1">
-        <f t="shared" ref="S13" si="5">Q13*1.2</f>
-        <v>60</v>
-      </c>
-      <c r="T13" s="1">
-        <v>50</v>
-      </c>
-      <c r="U13" s="1">
-        <f t="shared" ref="U13:U30" si="6">T13*0.8</f>
-        <v>40</v>
-      </c>
-      <c r="V13" s="1">
-        <f t="shared" ref="V13:V30" si="7">T13*1.2</f>
-        <v>60</v>
-      </c>
-      <c r="W13" s="1">
-        <v>50</v>
-      </c>
-      <c r="X13" s="1">
-        <f t="shared" ref="X13:X30" si="8">W13*0.8</f>
-        <v>40</v>
-      </c>
-      <c r="Y13" s="1">
-        <f t="shared" ref="Y13" si="9">W13*1.2</f>
-        <v>60</v>
-      </c>
-      <c r="Z13" s="1">
-        <v>50</v>
-      </c>
-      <c r="AA13" s="1">
-        <f t="shared" ref="AA13:AA30" si="10">Z13*0.8</f>
-        <v>40</v>
-      </c>
-      <c r="AB13" s="1">
-        <f t="shared" ref="AB13" si="11">Z13*1.2</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="1">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>0</v>
-      </c>
-      <c r="T14" s="1">
-        <v>0</v>
-      </c>
-      <c r="W14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0</v>
-      </c>
-      <c r="N15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>0</v>
-      </c>
-      <c r="T15" s="1">
-        <v>0</v>
-      </c>
-      <c r="W15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1813,10 +1760,10 @@
         <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>23</v>
@@ -1824,33 +1771,80 @@
       <c r="G16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="1" t="s">
-        <v>33</v>
+      <c r="H16" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="K16" s="1">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" ref="L16:L33" si="0">K16*0.8</f>
+        <v>40</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" ref="M16" si="1">K16*1.2</f>
+        <v>60</v>
       </c>
       <c r="N16" s="1">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" ref="O16:O33" si="2">N16*0.8</f>
+        <v>40</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" ref="P16" si="3">N16*1.2</f>
+        <v>60</v>
       </c>
       <c r="Q16" s="1">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="R16" s="1">
+        <f t="shared" ref="R16:R33" si="4">Q16*0.8</f>
+        <v>40</v>
+      </c>
+      <c r="S16" s="1">
+        <f t="shared" ref="S16" si="5">Q16*1.2</f>
+        <v>60</v>
       </c>
       <c r="T16" s="1">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="U16" s="1">
+        <f t="shared" ref="U16:U33" si="6">T16*0.8</f>
+        <v>40</v>
+      </c>
+      <c r="V16" s="1">
+        <f t="shared" ref="V16:V33" si="7">T16*1.2</f>
+        <v>60</v>
       </c>
       <c r="W16" s="1">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="X16" s="1">
+        <f t="shared" ref="X16:X33" si="8">W16*0.8</f>
+        <v>40</v>
+      </c>
+      <c r="Y16" s="1">
+        <f t="shared" ref="Y16" si="9">W16*1.2</f>
+        <v>60</v>
       </c>
       <c r="Z16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="AA16" s="1">
+        <f t="shared" ref="AA16:AA33" si="10">Z16*0.8</f>
+        <v>40</v>
+      </c>
+      <c r="AB16" s="1">
+        <f t="shared" ref="AB16" si="11">Z16*1.2</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1861,7 +1855,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>29</v>
@@ -1880,25 +1874,25 @@
         <v>10</v>
       </c>
       <c r="K17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1909,7 +1903,7 @@
         <v>19</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>29</v>
@@ -1946,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1957,7 +1951,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>29</v>
@@ -1994,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -2005,7 +1999,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>29</v>
@@ -2042,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -2053,7 +2047,7 @@
         <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>29</v>
@@ -2090,7 +2084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -2101,7 +2095,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>29</v>
@@ -2138,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -2149,7 +2143,7 @@
         <v>19</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>29</v>
@@ -2186,7 +2180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -2197,7 +2191,7 @@
         <v>19</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>29</v>
@@ -2216,25 +2210,25 @@
         <v>10</v>
       </c>
       <c r="K24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -2245,7 +2239,7 @@
         <v>19</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>29</v>
@@ -2264,25 +2258,25 @@
         <v>10</v>
       </c>
       <c r="K25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -2293,7 +2287,7 @@
         <v>19</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>29</v>
@@ -2312,39 +2306,39 @@
         <v>10</v>
       </c>
       <c r="K26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z26" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>23</v>
@@ -2352,526 +2346,526 @@
       <c r="G27" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H27" s="5"/>
       <c r="I27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>1</v>
+      </c>
+      <c r="T27" s="1">
+        <v>1</v>
+      </c>
+      <c r="W27" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="5"/>
+      <c r="I28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>0</v>
+      </c>
+      <c r="T28" s="1">
+        <v>0</v>
+      </c>
+      <c r="W28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0</v>
+      </c>
+      <c r="T29" s="1">
+        <v>0</v>
+      </c>
+      <c r="W29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K30" s="1">
         <v>50</v>
       </c>
-      <c r="L27" s="1">
+      <c r="L30" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="M27" s="1">
-        <f t="shared" ref="M27" si="12">K27*1.2</f>
+      <c r="M30" s="1">
+        <f t="shared" ref="M30" si="12">K30*1.2</f>
         <v>60</v>
       </c>
-      <c r="N27" s="1">
+      <c r="N30" s="1">
         <v>50</v>
       </c>
-      <c r="O27" s="1">
+      <c r="O30" s="1">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="P27" s="1">
-        <f t="shared" ref="P27" si="13">N27*1.2</f>
+      <c r="P30" s="1">
+        <f t="shared" ref="P30" si="13">N30*1.2</f>
         <v>60</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="Q30" s="1">
         <v>50</v>
       </c>
-      <c r="R27" s="1">
+      <c r="R30" s="1">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="S27" s="1">
-        <f t="shared" ref="S27" si="14">Q27*1.2</f>
+      <c r="S30" s="1">
+        <f t="shared" ref="S30" si="14">Q30*1.2</f>
         <v>60</v>
       </c>
-      <c r="T27" s="1">
+      <c r="T30" s="1">
         <v>50</v>
       </c>
-      <c r="U27" s="1">
+      <c r="U30" s="1">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="V27" s="1">
+      <c r="V30" s="1">
         <f t="shared" si="7"/>
         <v>60</v>
       </c>
-      <c r="W27" s="1">
+      <c r="W30" s="1">
         <v>50</v>
       </c>
-      <c r="X27" s="1">
+      <c r="X30" s="1">
         <f t="shared" si="8"/>
         <v>40</v>
       </c>
-      <c r="Y27" s="1">
-        <f t="shared" ref="Y27" si="15">W27*1.2</f>
+      <c r="Y30" s="1">
+        <f t="shared" ref="Y30" si="15">W30*1.2</f>
         <v>60</v>
       </c>
-      <c r="Z27" s="1">
+      <c r="Z30" s="1">
         <v>50</v>
       </c>
-      <c r="AA27" s="1">
+      <c r="AA30" s="1">
         <f t="shared" si="10"/>
         <v>40</v>
       </c>
-      <c r="AB27" s="1">
-        <f t="shared" ref="AB27" si="16">Z27*1.2</f>
+      <c r="AB30" s="1">
+        <f t="shared" ref="AB30" si="16">Z30*1.2</f>
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="C31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I28" s="1" t="s">
+      <c r="G31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K31" s="1">
         <v>50</v>
       </c>
-      <c r="L28" s="1">
+      <c r="L31" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="M28" s="1">
-        <f t="shared" ref="M28:M29" si="17">K28*1.2</f>
+      <c r="M31" s="1">
+        <f t="shared" ref="M31:M32" si="17">K31*1.2</f>
         <v>60</v>
       </c>
-      <c r="N28" s="1">
+      <c r="N31" s="1">
         <v>50</v>
       </c>
-      <c r="O28" s="1">
+      <c r="O31" s="1">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="P28" s="1">
-        <f t="shared" ref="P28:P29" si="18">N28*1.2</f>
+      <c r="P31" s="1">
+        <f t="shared" ref="P31:P32" si="18">N31*1.2</f>
         <v>60</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="Q31" s="1">
         <v>50</v>
       </c>
-      <c r="R28" s="1">
+      <c r="R31" s="1">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="S28" s="1">
-        <f t="shared" ref="S28:S29" si="19">Q28*1.2</f>
+      <c r="S31" s="1">
+        <f t="shared" ref="S31:S32" si="19">Q31*1.2</f>
         <v>60</v>
       </c>
-      <c r="T28" s="1">
+      <c r="T31" s="1">
         <v>50</v>
       </c>
-      <c r="U28" s="1">
+      <c r="U31" s="1">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="V28" s="1">
+      <c r="V31" s="1">
         <f t="shared" si="7"/>
         <v>60</v>
       </c>
-      <c r="W28" s="1">
+      <c r="W31" s="1">
         <v>50</v>
       </c>
-      <c r="X28" s="1">
+      <c r="X31" s="1">
         <f t="shared" si="8"/>
         <v>40</v>
       </c>
-      <c r="Y28" s="1">
-        <f t="shared" ref="Y28:Y29" si="20">W28*1.2</f>
+      <c r="Y31" s="1">
+        <f t="shared" ref="Y31:Y32" si="20">W31*1.2</f>
         <v>60</v>
       </c>
-      <c r="Z28" s="1">
+      <c r="Z31" s="1">
         <v>50</v>
       </c>
-      <c r="AA28" s="1">
+      <c r="AA31" s="1">
         <f t="shared" si="10"/>
         <v>40</v>
       </c>
-      <c r="AB28" s="1">
-        <f t="shared" ref="AB28:AB29" si="21">Z28*1.2</f>
+      <c r="AB31" s="1">
+        <f t="shared" ref="AB31:AB32" si="21">Z31*1.2</f>
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H29" s="5" t="s">
+      <c r="G32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K32" s="1">
         <f>2160/30</f>
         <v>72</v>
       </c>
-      <c r="L29" s="1">
+      <c r="L32" s="1">
         <f t="shared" si="0"/>
         <v>57.6</v>
       </c>
-      <c r="M29" s="1">
+      <c r="M32" s="1">
         <f t="shared" si="17"/>
         <v>86.399999999999991</v>
       </c>
-      <c r="N29" s="1">
+      <c r="N32" s="1">
         <f>2160/30</f>
         <v>72</v>
       </c>
-      <c r="O29" s="1">
+      <c r="O32" s="1">
         <f t="shared" si="2"/>
         <v>57.6</v>
       </c>
-      <c r="P29" s="1">
+      <c r="P32" s="1">
         <f t="shared" si="18"/>
         <v>86.399999999999991</v>
       </c>
-      <c r="Q29" s="1">
+      <c r="Q32" s="1">
         <f>2160/30</f>
         <v>72</v>
       </c>
-      <c r="R29" s="1">
+      <c r="R32" s="1">
         <f t="shared" si="4"/>
         <v>57.6</v>
       </c>
-      <c r="S29" s="1">
+      <c r="S32" s="1">
         <f t="shared" si="19"/>
         <v>86.399999999999991</v>
       </c>
-      <c r="T29" s="1">
+      <c r="T32" s="1">
         <f>2160/30</f>
         <v>72</v>
       </c>
-      <c r="U29" s="1">
+      <c r="U32" s="1">
         <f t="shared" si="6"/>
         <v>57.6</v>
       </c>
-      <c r="V29" s="1">
+      <c r="V32" s="1">
         <f t="shared" si="7"/>
         <v>86.399999999999991</v>
       </c>
-      <c r="W29" s="1">
+      <c r="W32" s="1">
         <f>2160/30</f>
         <v>72</v>
       </c>
-      <c r="X29" s="1">
+      <c r="X32" s="1">
         <f t="shared" si="8"/>
         <v>57.6</v>
       </c>
-      <c r="Y29" s="1">
+      <c r="Y32" s="1">
         <f t="shared" si="20"/>
         <v>86.399999999999991</v>
       </c>
-      <c r="Z29" s="1">
+      <c r="Z32" s="1">
         <f>2160/30</f>
         <v>72</v>
       </c>
-      <c r="AA29" s="1">
+      <c r="AA32" s="1">
         <f t="shared" si="10"/>
         <v>57.6</v>
       </c>
-      <c r="AB29" s="1">
+      <c r="AB32" s="1">
         <f t="shared" si="21"/>
         <v>86.399999999999991</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" s="5" t="s">
+      <c r="G33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K33" s="1">
         <v>600</v>
       </c>
-      <c r="L30" s="1">
+      <c r="L33" s="1">
         <f t="shared" si="0"/>
         <v>480</v>
       </c>
-      <c r="M30" s="1">
-        <f t="shared" ref="M30" si="22">K30*1.2</f>
+      <c r="M33" s="1">
+        <f t="shared" ref="M33" si="22">K33*1.2</f>
         <v>720</v>
       </c>
-      <c r="N30" s="1">
+      <c r="N33" s="1">
         <v>2160</v>
       </c>
-      <c r="O30" s="1">
+      <c r="O33" s="1">
         <f t="shared" si="2"/>
         <v>1728</v>
       </c>
-      <c r="P30" s="1">
-        <f t="shared" ref="P30" si="23">N30*1.2</f>
+      <c r="P33" s="1">
+        <f t="shared" ref="P33" si="23">N33*1.2</f>
         <v>2592</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="Q33" s="1">
         <v>2160</v>
       </c>
-      <c r="R30" s="1">
+      <c r="R33" s="1">
         <f t="shared" si="4"/>
         <v>1728</v>
       </c>
-      <c r="S30" s="1">
-        <f t="shared" ref="S30" si="24">Q30*1.2</f>
+      <c r="S33" s="1">
+        <f t="shared" ref="S33" si="24">Q33*1.2</f>
         <v>2592</v>
       </c>
-      <c r="T30" s="1">
+      <c r="T33" s="1">
         <v>2160</v>
       </c>
-      <c r="U30" s="1">
+      <c r="U33" s="1">
         <f t="shared" si="6"/>
         <v>1728</v>
       </c>
-      <c r="V30" s="1">
+      <c r="V33" s="1">
         <f t="shared" si="7"/>
         <v>2592</v>
       </c>
-      <c r="W30" s="1">
+      <c r="W33" s="1">
         <v>2160</v>
       </c>
-      <c r="X30" s="1">
+      <c r="X33" s="1">
         <f t="shared" si="8"/>
         <v>1728</v>
       </c>
-      <c r="Y30" s="1">
-        <f t="shared" ref="Y30" si="25">W30*1.2</f>
+      <c r="Y33" s="1">
+        <f t="shared" ref="Y33" si="25">W33*1.2</f>
         <v>2592</v>
       </c>
-      <c r="Z30" s="1">
+      <c r="Z33" s="1">
         <v>2160</v>
       </c>
-      <c r="AA30" s="1">
+      <c r="AA33" s="1">
         <f t="shared" si="10"/>
         <v>1728</v>
       </c>
-      <c r="AB30" s="1">
-        <f t="shared" ref="AB30" si="26">Z30*1.2</f>
+      <c r="AB33" s="1">
+        <f t="shared" ref="AB33" si="26">Z33*1.2</f>
         <v>2592</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K31" s="1">
-        <v>0</v>
-      </c>
-      <c r="N31" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="1">
-        <v>0</v>
-      </c>
-      <c r="T31" s="1">
-        <v>0</v>
-      </c>
-      <c r="W31" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32" s="5"/>
-      <c r="I32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K32" s="1">
-        <v>0</v>
-      </c>
-      <c r="N32" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="1">
-        <v>0</v>
-      </c>
-      <c r="T32" s="1">
-        <v>0</v>
-      </c>
-      <c r="W32" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H33" s="5"/>
-      <c r="I33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K33" s="1">
-        <v>0</v>
-      </c>
-      <c r="N33" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="1">
-        <v>0</v>
-      </c>
-      <c r="T33" s="1">
-        <v>0</v>
-      </c>
-      <c r="W33" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>29</v>
@@ -2890,39 +2884,39 @@
         <v>10</v>
       </c>
       <c r="K34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>23</v>
@@ -2930,82 +2924,35 @@
       <c r="G35" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H35" s="5"/>
       <c r="I35" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="K35" s="1">
-        <v>2400</v>
-      </c>
-      <c r="L35" s="1">
-        <f t="shared" ref="L35:L43" si="27">K35*0.9</f>
-        <v>2160</v>
-      </c>
-      <c r="M35" s="1">
-        <f t="shared" ref="M35:M43" si="28">K35*1.1</f>
-        <v>2640</v>
+        <v>0</v>
       </c>
       <c r="N35" s="1">
-        <v>2400</v>
-      </c>
-      <c r="O35" s="1">
-        <f t="shared" ref="O35:O43" si="29">N35*0.9</f>
-        <v>2160</v>
-      </c>
-      <c r="P35" s="1">
-        <f t="shared" ref="P35:P43" si="30">N35*1.1</f>
-        <v>2640</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="1">
-        <v>2400</v>
-      </c>
-      <c r="R35" s="1">
-        <f t="shared" ref="R35:R43" si="31">Q35*0.9</f>
-        <v>2160</v>
-      </c>
-      <c r="S35" s="1">
-        <f t="shared" ref="S35:S43" si="32">Q35*1.1</f>
-        <v>2640</v>
+        <v>0</v>
       </c>
       <c r="T35" s="1">
-        <v>2400</v>
-      </c>
-      <c r="U35" s="1">
-        <f t="shared" ref="U35:U42" si="33">T35*0.9</f>
-        <v>2160</v>
-      </c>
-      <c r="V35" s="1">
-        <f t="shared" ref="V35:V42" si="34">T35*1.1</f>
-        <v>2640</v>
+        <v>0</v>
       </c>
       <c r="W35" s="1">
-        <v>2400</v>
-      </c>
-      <c r="X35" s="1">
-        <f t="shared" ref="X35:X43" si="35">W35*0.9</f>
-        <v>2160</v>
-      </c>
-      <c r="Y35" s="1">
-        <f t="shared" ref="Y35:Y43" si="36">W35*1.1</f>
-        <v>2640</v>
+        <v>0</v>
       </c>
       <c r="Z35" s="1">
-        <v>2400</v>
-      </c>
-      <c r="AA35" s="1">
-        <f t="shared" ref="AA35:AA43" si="37">Z35*0.9</f>
-        <v>2160</v>
-      </c>
-      <c r="AB35" s="1">
-        <f t="shared" ref="AB35:AB43" si="38">Z35*1.1</f>
-        <v>2640</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>20</v>
@@ -3014,10 +2961,10 @@
         <v>19</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>23</v>
@@ -3025,692 +2972,883 @@
       <c r="G36" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H36" s="5"/>
       <c r="I36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>0</v>
+      </c>
+      <c r="T36" s="1">
+        <v>0</v>
+      </c>
+      <c r="W36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="5"/>
+      <c r="I37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K37" s="1">
+        <v>1</v>
+      </c>
+      <c r="N37" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>1</v>
+      </c>
+      <c r="T37" s="1">
+        <v>1</v>
+      </c>
+      <c r="W37" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K38" s="1">
+        <v>2400</v>
+      </c>
+      <c r="L38" s="1">
+        <f t="shared" ref="L38:L45" si="27">K38*0.9</f>
+        <v>2160</v>
+      </c>
+      <c r="M38" s="1">
+        <f t="shared" ref="M38:M45" si="28">K38*1.1</f>
+        <v>2640</v>
+      </c>
+      <c r="N38" s="1">
+        <v>2400</v>
+      </c>
+      <c r="O38" s="1">
+        <f t="shared" ref="O38:O45" si="29">N38*0.9</f>
+        <v>2160</v>
+      </c>
+      <c r="P38" s="1">
+        <f t="shared" ref="P38:P45" si="30">N38*1.1</f>
+        <v>2640</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>2400</v>
+      </c>
+      <c r="R38" s="1">
+        <f t="shared" ref="R38:R45" si="31">Q38*0.9</f>
+        <v>2160</v>
+      </c>
+      <c r="S38" s="1">
+        <f t="shared" ref="S38:S45" si="32">Q38*1.1</f>
+        <v>2640</v>
+      </c>
+      <c r="T38" s="1">
+        <v>2400</v>
+      </c>
+      <c r="U38" s="1">
+        <f t="shared" ref="U38:U45" si="33">T38*0.9</f>
+        <v>2160</v>
+      </c>
+      <c r="V38" s="1">
+        <f t="shared" ref="V38:V45" si="34">T38*1.1</f>
+        <v>2640</v>
+      </c>
+      <c r="W38" s="1">
+        <v>2400</v>
+      </c>
+      <c r="X38" s="1">
+        <f t="shared" ref="X38:X45" si="35">W38*0.9</f>
+        <v>2160</v>
+      </c>
+      <c r="Y38" s="1">
+        <f t="shared" ref="Y38:Y45" si="36">W38*1.1</f>
+        <v>2640</v>
+      </c>
+      <c r="Z38" s="1">
+        <v>2400</v>
+      </c>
+      <c r="AA38" s="1">
+        <f t="shared" ref="AA38:AA45" si="37">Z38*0.9</f>
+        <v>2160</v>
+      </c>
+      <c r="AB38" s="1">
+        <f t="shared" ref="AB38:AB45" si="38">Z38*1.1</f>
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K39" s="1">
         <v>300</v>
       </c>
-      <c r="L36" s="1">
+      <c r="L39" s="1">
         <f t="shared" si="27"/>
         <v>270</v>
       </c>
-      <c r="M36" s="1">
+      <c r="M39" s="1">
         <f t="shared" si="28"/>
         <v>330</v>
       </c>
-      <c r="N36" s="1">
+      <c r="N39" s="1">
         <v>300</v>
       </c>
-      <c r="O36" s="1">
+      <c r="O39" s="1">
         <f t="shared" si="29"/>
         <v>270</v>
       </c>
-      <c r="P36" s="1">
+      <c r="P39" s="1">
         <f t="shared" si="30"/>
         <v>330</v>
       </c>
-      <c r="Q36" s="1">
+      <c r="Q39" s="1">
         <v>300</v>
       </c>
-      <c r="R36" s="1">
+      <c r="R39" s="1">
         <f t="shared" si="31"/>
         <v>270</v>
       </c>
-      <c r="S36" s="1">
+      <c r="S39" s="1">
         <f t="shared" si="32"/>
         <v>330</v>
       </c>
-      <c r="T36" s="1">
+      <c r="T39" s="1">
         <v>300</v>
       </c>
-      <c r="U36" s="1">
+      <c r="U39" s="1">
         <f t="shared" si="33"/>
         <v>270</v>
       </c>
-      <c r="V36" s="1">
+      <c r="V39" s="1">
         <f t="shared" si="34"/>
         <v>330</v>
       </c>
-      <c r="W36" s="1">
+      <c r="W39" s="1">
         <v>300</v>
       </c>
-      <c r="X36" s="1">
+      <c r="X39" s="1">
         <f t="shared" si="35"/>
         <v>270</v>
       </c>
-      <c r="Y36" s="1">
+      <c r="Y39" s="1">
         <f t="shared" si="36"/>
         <v>330</v>
       </c>
-      <c r="Z36" s="1">
+      <c r="Z39" s="1">
         <v>300</v>
       </c>
-      <c r="AA36" s="1">
+      <c r="AA39" s="1">
         <f t="shared" si="37"/>
         <v>270</v>
       </c>
-      <c r="AB36" s="1">
+      <c r="AB39" s="1">
         <f t="shared" si="38"/>
         <v>330</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="C40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="1" t="s">
+      <c r="G40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K40" s="1">
         <v>300</v>
       </c>
-      <c r="L37" s="1">
+      <c r="L40" s="1">
         <f t="shared" si="27"/>
         <v>270</v>
       </c>
-      <c r="M37" s="1">
+      <c r="M40" s="1">
         <f t="shared" si="28"/>
         <v>330</v>
       </c>
-      <c r="N37" s="1">
+      <c r="N40" s="1">
         <v>300</v>
       </c>
-      <c r="O37" s="1">
+      <c r="O40" s="1">
         <f t="shared" si="29"/>
         <v>270</v>
       </c>
-      <c r="P37" s="1">
+      <c r="P40" s="1">
         <f t="shared" si="30"/>
         <v>330</v>
       </c>
-      <c r="Q37" s="1">
+      <c r="Q40" s="1">
         <v>300</v>
       </c>
-      <c r="R37" s="1">
+      <c r="R40" s="1">
         <f t="shared" si="31"/>
         <v>270</v>
       </c>
-      <c r="S37" s="1">
+      <c r="S40" s="1">
         <f t="shared" si="32"/>
         <v>330</v>
       </c>
-      <c r="T37" s="1">
+      <c r="T40" s="1">
         <v>300</v>
       </c>
-      <c r="U37" s="1">
+      <c r="U40" s="1">
         <f t="shared" si="33"/>
         <v>270</v>
       </c>
-      <c r="V37" s="1">
+      <c r="V40" s="1">
         <f t="shared" si="34"/>
         <v>330</v>
       </c>
-      <c r="W37" s="1">
+      <c r="W40" s="1">
         <v>300</v>
       </c>
-      <c r="X37" s="1">
+      <c r="X40" s="1">
         <f t="shared" si="35"/>
         <v>270</v>
       </c>
-      <c r="Y37" s="1">
+      <c r="Y40" s="1">
         <f t="shared" si="36"/>
         <v>330</v>
       </c>
-      <c r="Z37" s="1">
+      <c r="Z40" s="1">
         <v>300</v>
       </c>
-      <c r="AA37" s="1">
+      <c r="AA40" s="1">
         <f t="shared" si="37"/>
         <v>270</v>
       </c>
-      <c r="AB37" s="1">
+      <c r="AB40" s="1">
         <f t="shared" si="38"/>
         <v>330</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="C41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K41" s="1">
         <v>20</v>
       </c>
-      <c r="L38" s="1">
+      <c r="L41" s="1">
         <f t="shared" si="27"/>
         <v>18</v>
       </c>
-      <c r="M38" s="1">
+      <c r="M41" s="1">
         <f t="shared" si="28"/>
         <v>22</v>
       </c>
-      <c r="N38" s="1">
+      <c r="N41" s="1">
         <v>20</v>
       </c>
-      <c r="O38" s="1">
+      <c r="O41" s="1">
         <f t="shared" si="29"/>
         <v>18</v>
       </c>
-      <c r="P38" s="1">
+      <c r="P41" s="1">
         <f t="shared" si="30"/>
         <v>22</v>
       </c>
-      <c r="Q38" s="1">
+      <c r="Q41" s="1">
         <v>20</v>
       </c>
-      <c r="R38" s="1">
+      <c r="R41" s="1">
         <f t="shared" si="31"/>
         <v>18</v>
       </c>
-      <c r="S38" s="1">
+      <c r="S41" s="1">
         <f t="shared" si="32"/>
         <v>22</v>
       </c>
-      <c r="T38" s="1">
+      <c r="T41" s="1">
         <v>20</v>
       </c>
-      <c r="U38" s="1">
+      <c r="U41" s="1">
         <f t="shared" si="33"/>
         <v>18</v>
       </c>
-      <c r="V38" s="1">
+      <c r="V41" s="1">
         <f t="shared" si="34"/>
         <v>22</v>
       </c>
-      <c r="W38" s="1">
+      <c r="W41" s="1">
         <v>20</v>
       </c>
-      <c r="X38" s="1">
+      <c r="X41" s="1">
         <f t="shared" si="35"/>
         <v>18</v>
       </c>
-      <c r="Y38" s="1">
+      <c r="Y41" s="1">
         <f t="shared" si="36"/>
         <v>22</v>
       </c>
-      <c r="Z38" s="1">
+      <c r="Z41" s="1">
         <v>20</v>
       </c>
-      <c r="AA38" s="1">
+      <c r="AA41" s="1">
         <f t="shared" si="37"/>
         <v>18</v>
       </c>
-      <c r="AB38" s="1">
+      <c r="AB41" s="1">
         <f t="shared" si="38"/>
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="C42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K39" s="1">
+      <c r="K42" s="1">
         <v>25</v>
       </c>
-      <c r="L39" s="1">
+      <c r="L42" s="1">
         <f t="shared" si="27"/>
         <v>22.5</v>
       </c>
-      <c r="M39" s="1">
+      <c r="M42" s="1">
         <f t="shared" si="28"/>
         <v>27.500000000000004</v>
       </c>
-      <c r="N39" s="1">
+      <c r="N42" s="1">
         <v>25</v>
       </c>
-      <c r="O39" s="1">
+      <c r="O42" s="1">
         <f t="shared" si="29"/>
         <v>22.5</v>
       </c>
-      <c r="P39" s="1">
+      <c r="P42" s="1">
         <f t="shared" si="30"/>
         <v>27.500000000000004</v>
       </c>
-      <c r="Q39" s="1">
+      <c r="Q42" s="1">
         <v>25</v>
       </c>
-      <c r="R39" s="1">
+      <c r="R42" s="1">
         <f t="shared" si="31"/>
         <v>22.5</v>
       </c>
-      <c r="S39" s="1">
+      <c r="S42" s="1">
         <f t="shared" si="32"/>
         <v>27.500000000000004</v>
       </c>
-      <c r="T39" s="1">
+      <c r="T42" s="1">
         <v>25</v>
       </c>
-      <c r="U39" s="1">
+      <c r="U42" s="1">
         <f t="shared" si="33"/>
         <v>22.5</v>
       </c>
-      <c r="V39" s="1">
+      <c r="V42" s="1">
         <f t="shared" si="34"/>
         <v>27.500000000000004</v>
       </c>
-      <c r="W39" s="1">
+      <c r="W42" s="1">
         <v>25</v>
       </c>
-      <c r="X39" s="1">
+      <c r="X42" s="1">
         <f t="shared" si="35"/>
         <v>22.5</v>
       </c>
-      <c r="Y39" s="1">
+      <c r="Y42" s="1">
         <f t="shared" si="36"/>
         <v>27.500000000000004</v>
       </c>
-      <c r="Z39" s="1">
+      <c r="Z42" s="1">
         <v>25</v>
       </c>
-      <c r="AA39" s="1">
+      <c r="AA42" s="1">
         <f t="shared" si="37"/>
         <v>22.5</v>
       </c>
-      <c r="AB39" s="1">
+      <c r="AB42" s="1">
         <f t="shared" si="38"/>
         <v>27.500000000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="C43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K43" s="1">
         <v>5</v>
       </c>
-      <c r="L40" s="1">
+      <c r="L43" s="1">
         <f t="shared" si="27"/>
         <v>4.5</v>
       </c>
-      <c r="M40" s="1">
+      <c r="M43" s="1">
         <f t="shared" si="28"/>
         <v>5.5</v>
       </c>
-      <c r="N40" s="1">
+      <c r="N43" s="1">
         <v>5</v>
       </c>
-      <c r="O40" s="1">
+      <c r="O43" s="1">
         <f t="shared" si="29"/>
         <v>4.5</v>
       </c>
-      <c r="P40" s="1">
+      <c r="P43" s="1">
         <f t="shared" si="30"/>
         <v>5.5</v>
       </c>
-      <c r="Q40" s="1">
+      <c r="Q43" s="1">
         <v>5</v>
       </c>
-      <c r="R40" s="1">
+      <c r="R43" s="1">
         <f t="shared" si="31"/>
         <v>4.5</v>
       </c>
-      <c r="S40" s="1">
+      <c r="S43" s="1">
         <f t="shared" si="32"/>
         <v>5.5</v>
       </c>
-      <c r="T40" s="1">
+      <c r="T43" s="1">
         <v>5</v>
       </c>
-      <c r="U40" s="1">
+      <c r="U43" s="1">
         <f t="shared" si="33"/>
         <v>4.5</v>
       </c>
-      <c r="V40" s="1">
+      <c r="V43" s="1">
         <f t="shared" si="34"/>
         <v>5.5</v>
       </c>
-      <c r="W40" s="1">
+      <c r="W43" s="1">
         <v>5</v>
       </c>
-      <c r="X40" s="1">
+      <c r="X43" s="1">
         <f t="shared" si="35"/>
         <v>4.5</v>
       </c>
-      <c r="Y40" s="1">
+      <c r="Y43" s="1">
         <f t="shared" si="36"/>
         <v>5.5</v>
       </c>
-      <c r="Z40" s="1">
+      <c r="Z43" s="1">
         <v>5</v>
       </c>
-      <c r="AA40" s="1">
+      <c r="AA43" s="1">
         <f t="shared" si="37"/>
         <v>4.5</v>
       </c>
-      <c r="AB40" s="1">
+      <c r="AB43" s="1">
         <f t="shared" si="38"/>
         <v>5.5</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K44" s="1">
         <v>50</v>
       </c>
-      <c r="L41" s="1">
+      <c r="L44" s="1">
         <f t="shared" si="27"/>
         <v>45</v>
       </c>
-      <c r="M41" s="1">
+      <c r="M44" s="1">
         <f t="shared" si="28"/>
         <v>55.000000000000007</v>
       </c>
-      <c r="N41" s="1">
+      <c r="N44" s="1">
         <v>50</v>
       </c>
-      <c r="O41" s="1">
+      <c r="O44" s="1">
         <f t="shared" si="29"/>
         <v>45</v>
       </c>
-      <c r="P41" s="1">
+      <c r="P44" s="1">
         <f t="shared" si="30"/>
         <v>55.000000000000007</v>
       </c>
-      <c r="Q41" s="1">
+      <c r="Q44" s="1">
         <v>50</v>
       </c>
-      <c r="R41" s="1">
+      <c r="R44" s="1">
         <f t="shared" si="31"/>
         <v>45</v>
       </c>
-      <c r="S41" s="1">
+      <c r="S44" s="1">
         <f t="shared" si="32"/>
         <v>55.000000000000007</v>
       </c>
-      <c r="T41" s="1">
+      <c r="T44" s="1">
         <v>50</v>
       </c>
-      <c r="U41" s="1">
+      <c r="U44" s="1">
         <f t="shared" si="33"/>
         <v>45</v>
       </c>
-      <c r="V41" s="1">
+      <c r="V44" s="1">
         <f t="shared" si="34"/>
         <v>55.000000000000007</v>
       </c>
-      <c r="W41" s="1">
+      <c r="W44" s="1">
         <v>50</v>
       </c>
-      <c r="X41" s="1">
+      <c r="X44" s="1">
         <f t="shared" si="35"/>
         <v>45</v>
       </c>
-      <c r="Y41" s="1">
+      <c r="Y44" s="1">
         <f t="shared" si="36"/>
         <v>55.000000000000007</v>
       </c>
-      <c r="Z41" s="1">
+      <c r="Z44" s="1">
         <v>50</v>
       </c>
-      <c r="AA41" s="1">
+      <c r="AA44" s="1">
         <f t="shared" si="37"/>
         <v>45</v>
       </c>
-      <c r="AB41" s="1">
+      <c r="AB44" s="1">
         <f t="shared" si="38"/>
         <v>55.000000000000007</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="C45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="J45" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K42" s="1">
+      <c r="K45" s="1">
         <v>500</v>
       </c>
-      <c r="L42" s="1">
+      <c r="L45" s="1">
         <f t="shared" si="27"/>
         <v>450</v>
       </c>
-      <c r="M42" s="1">
+      <c r="M45" s="1">
         <f t="shared" si="28"/>
         <v>550</v>
       </c>
-      <c r="N42" s="1">
+      <c r="N45" s="1">
         <v>500</v>
       </c>
-      <c r="O42" s="1">
+      <c r="O45" s="1">
         <f t="shared" si="29"/>
         <v>450</v>
       </c>
-      <c r="P42" s="1">
+      <c r="P45" s="1">
         <f t="shared" si="30"/>
         <v>550</v>
       </c>
-      <c r="Q42" s="1">
+      <c r="Q45" s="1">
         <v>500</v>
       </c>
-      <c r="R42" s="1">
+      <c r="R45" s="1">
         <f t="shared" si="31"/>
         <v>450</v>
       </c>
-      <c r="S42" s="1">
+      <c r="S45" s="1">
         <f t="shared" si="32"/>
         <v>550</v>
       </c>
-      <c r="T42" s="1">
+      <c r="T45" s="1">
         <v>500</v>
       </c>
-      <c r="U42" s="1">
+      <c r="U45" s="1">
         <f t="shared" si="33"/>
         <v>450</v>
       </c>
-      <c r="V42" s="1">
+      <c r="V45" s="1">
         <f t="shared" si="34"/>
         <v>550</v>
       </c>
-      <c r="W42" s="1">
+      <c r="W45" s="1">
         <v>500</v>
       </c>
-      <c r="X42" s="1">
+      <c r="X45" s="1">
         <f t="shared" si="35"/>
         <v>450</v>
       </c>
-      <c r="Y42" s="1">
+      <c r="Y45" s="1">
         <f t="shared" si="36"/>
         <v>550</v>
       </c>
-      <c r="Z42" s="1">
+      <c r="Z45" s="1">
         <v>500</v>
       </c>
-      <c r="AA42" s="1">
+      <c r="AA45" s="1">
         <f t="shared" si="37"/>
         <v>450</v>
       </c>
-      <c r="AB42" s="1">
+      <c r="AB45" s="1">
         <f t="shared" si="38"/>
         <v>550</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="C46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K43" s="1">
-        <v>1</v>
-      </c>
-      <c r="N43" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q43" s="1">
-        <v>1</v>
-      </c>
-      <c r="T43" s="1">
-        <v>1</v>
-      </c>
-      <c r="W43" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z43" s="1">
+      <c r="K46" s="1">
+        <v>1</v>
+      </c>
+      <c r="N46" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>1</v>
+      </c>
+      <c r="T46" s="1">
+        <v>1</v>
+      </c>
+      <c r="W46" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z46" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:Y42" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:Y45" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update of new sizes.
</commit_message>
<xml_diff>
--- a/windisch/data/Input data.xlsx
+++ b/windisch/data/Input data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/windisch/windisch/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhuber\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3844C490-07BB-1B4E-9780-6ED29D64154B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B8B361-E618-4EC8-B967-3125460ABD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28420" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$2:$Y$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$2:$Y$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="79">
   <si>
     <t>parameter</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>power</t>
+  </si>
+  <si>
+    <t>10000kW</t>
+  </si>
+  <si>
+    <t>15000kW</t>
+  </si>
+  <si>
+    <t>3400kW</t>
   </si>
 </sst>
 </file>
@@ -368,9 +377,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -408,9 +417,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -443,26 +452,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -495,26 +487,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -688,42 +663,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB43"/>
+  <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="26.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="8.83203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="8.77734375" style="1" customWidth="1"/>
     <col min="23" max="23" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="29" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -809,7 +785,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -875,7 +851,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -929,7 +905,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -983,7 +959,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1037,7 +1013,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1091,7 +1067,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1099,7 +1075,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>75</v>
@@ -1117,319 +1093,211 @@
         <v>10</v>
       </c>
       <c r="K7" s="1">
-        <v>8000</v>
+        <v>3400</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="1">
-        <v>8000</v>
+        <v>3400</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="1">
-        <v>8000</v>
+        <v>3400</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="1">
-        <v>8000</v>
+        <v>3400</v>
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
       <c r="W7" s="1">
-        <v>8000</v>
+        <v>3400</v>
       </c>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
       <c r="Z7" s="1">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="1">
         <v>8000</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="1">
+        <v>8000</v>
+      </c>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="1">
+        <v>8000</v>
+      </c>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="1">
+        <v>8000</v>
+      </c>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="1">
+        <v>8000</v>
+      </c>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="1">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="1">
+        <v>15000</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="1">
+        <v>15000</v>
+      </c>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="1">
+        <v>15000</v>
+      </c>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="1">
+        <v>15000</v>
+      </c>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="1">
+        <v>15000</v>
+      </c>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="1">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" s="1">
-        <v>30</v>
-      </c>
-      <c r="L8" s="1">
-        <v>25</v>
-      </c>
-      <c r="M8" s="1">
-        <v>35</v>
-      </c>
-      <c r="N8" s="1">
-        <v>30</v>
-      </c>
-      <c r="O8" s="1">
-        <v>25</v>
-      </c>
-      <c r="P8" s="1">
-        <v>35</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>30</v>
-      </c>
-      <c r="R8" s="1">
-        <v>25</v>
-      </c>
-      <c r="S8" s="1">
-        <v>35</v>
-      </c>
-      <c r="T8" s="1">
-        <v>30</v>
-      </c>
-      <c r="U8" s="1">
-        <v>25</v>
-      </c>
-      <c r="V8" s="1">
-        <v>35</v>
-      </c>
-      <c r="W8" s="1">
-        <v>30</v>
-      </c>
-      <c r="X8" s="1">
-        <v>25</v>
-      </c>
-      <c r="Y8" s="1">
-        <v>35</v>
-      </c>
-      <c r="Z8" s="1">
-        <v>30</v>
-      </c>
-      <c r="AA8" s="1">
-        <v>25</v>
-      </c>
-      <c r="AB8" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="1">
-        <v>600</v>
-      </c>
-      <c r="L9" s="1">
-        <f>K9*0.8</f>
-        <v>480</v>
-      </c>
-      <c r="M9" s="1">
-        <f>K9*1.2</f>
-        <v>720</v>
-      </c>
-      <c r="N9" s="1">
-        <v>600</v>
-      </c>
-      <c r="O9" s="1">
-        <f>N9*0.8</f>
-        <v>480</v>
-      </c>
-      <c r="P9" s="1">
-        <f>N9*1.2</f>
-        <v>720</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>600</v>
-      </c>
-      <c r="R9" s="1">
-        <f>Q9*0.8</f>
-        <v>480</v>
-      </c>
-      <c r="S9" s="1">
-        <f>Q9*1.2</f>
-        <v>720</v>
-      </c>
-      <c r="T9" s="1">
-        <v>600</v>
-      </c>
-      <c r="U9" s="1">
-        <f>T9*0.8</f>
-        <v>480</v>
-      </c>
-      <c r="V9" s="1">
-        <f>T9*1.2</f>
-        <v>720</v>
-      </c>
-      <c r="W9" s="1">
-        <v>600</v>
-      </c>
-      <c r="X9" s="1">
-        <f>W9*0.8</f>
-        <v>480</v>
-      </c>
-      <c r="Y9" s="1">
-        <f>W9*1.2</f>
-        <v>720</v>
-      </c>
-      <c r="Z9" s="1">
-        <v>600</v>
-      </c>
-      <c r="AA9" s="1">
-        <f>Z9*0.8</f>
-        <v>480</v>
-      </c>
-      <c r="AB9" s="1">
-        <f>Z9*1.2</f>
-        <v>720</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K10" s="1">
-        <v>1025</v>
-      </c>
-      <c r="L10" s="1">
-        <f>K10*0.8</f>
-        <v>820</v>
-      </c>
-      <c r="M10" s="1">
-        <f>K10*1.2</f>
-        <v>1230</v>
-      </c>
-      <c r="N10" s="1">
-        <v>1025</v>
-      </c>
-      <c r="O10" s="1">
-        <f>N10*0.8</f>
-        <v>820</v>
-      </c>
-      <c r="P10" s="1">
-        <f>N10*1.2</f>
-        <v>1230</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>1025</v>
-      </c>
-      <c r="R10" s="1">
-        <f>Q10*0.8</f>
-        <v>820</v>
-      </c>
-      <c r="S10" s="1">
-        <f>Q10*1.2</f>
-        <v>1230</v>
-      </c>
-      <c r="T10" s="1">
-        <v>1025</v>
-      </c>
-      <c r="U10" s="1">
-        <f>T10*0.8</f>
-        <v>820</v>
-      </c>
-      <c r="V10" s="1">
-        <f>T10*1.2</f>
-        <v>1230</v>
-      </c>
-      <c r="W10" s="1">
-        <v>1025</v>
-      </c>
-      <c r="X10" s="1">
-        <f>W10*0.8</f>
-        <v>820</v>
-      </c>
-      <c r="Y10" s="1">
-        <f>W10*1.2</f>
-        <v>1230</v>
-      </c>
-      <c r="Z10" s="1">
-        <v>1025</v>
-      </c>
-      <c r="AA10" s="1">
-        <f>Z10*0.8</f>
-        <v>820</v>
-      </c>
-      <c r="AB10" s="1">
-        <f>Z10*1.2</f>
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>23</v>
@@ -1437,82 +1305,67 @@
       <c r="G11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="J11" s="1" t="s">
         <v>56</v>
       </c>
       <c r="K11" s="1">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="L11" s="1">
-        <f>K11*0.8</f>
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="M11" s="1">
-        <f>K11*1.2</f>
-        <v>720</v>
+        <v>35</v>
       </c>
       <c r="N11" s="1">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="O11" s="1">
-        <f>N11*0.8</f>
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="P11" s="1">
-        <f>N11*1.2</f>
-        <v>720</v>
+        <v>35</v>
       </c>
       <c r="Q11" s="1">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="R11" s="1">
-        <f>Q11*0.8</f>
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="S11" s="1">
-        <f>Q11*1.2</f>
-        <v>720</v>
+        <v>35</v>
       </c>
       <c r="T11" s="1">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="U11" s="1">
-        <f>T11*0.8</f>
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="V11" s="1">
-        <f>T11*1.2</f>
-        <v>720</v>
+        <v>35</v>
       </c>
       <c r="W11" s="1">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="X11" s="1">
-        <f>W11*0.8</f>
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="Y11" s="1">
-        <f>W11*1.2</f>
-        <v>720</v>
+        <v>35</v>
       </c>
       <c r="Z11" s="1">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="AA11" s="1">
-        <f>Z11*0.8</f>
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="AB11" s="1">
-        <f>Z11*1.2</f>
-        <v>720</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>19</v>
@@ -1521,7 +1374,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>9</v>
@@ -1539,270 +1392,364 @@
         <v>56</v>
       </c>
       <c r="K12" s="1">
+        <v>600</v>
+      </c>
+      <c r="L12" s="1">
+        <f>K12*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="M12" s="1">
+        <f>K12*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="N12" s="1">
+        <v>600</v>
+      </c>
+      <c r="O12" s="1">
+        <f>N12*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="P12" s="1">
+        <f>N12*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>600</v>
+      </c>
+      <c r="R12" s="1">
+        <f>Q12*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="S12" s="1">
+        <f>Q12*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="T12" s="1">
+        <v>600</v>
+      </c>
+      <c r="U12" s="1">
+        <f>T12*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="V12" s="1">
+        <f>T12*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="W12" s="1">
+        <v>600</v>
+      </c>
+      <c r="X12" s="1">
+        <f>W12*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="Y12" s="1">
+        <f>W12*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>600</v>
+      </c>
+      <c r="AA12" s="1">
+        <f>Z12*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="AB12" s="1">
+        <f>Z12*1.2</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1025</v>
+      </c>
+      <c r="L13" s="1">
+        <f>K13*0.8</f>
+        <v>820</v>
+      </c>
+      <c r="M13" s="1">
+        <f>K13*1.2</f>
+        <v>1230</v>
+      </c>
+      <c r="N13" s="1">
+        <v>1025</v>
+      </c>
+      <c r="O13" s="1">
+        <f>N13*0.8</f>
+        <v>820</v>
+      </c>
+      <c r="P13" s="1">
+        <f>N13*1.2</f>
+        <v>1230</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>1025</v>
+      </c>
+      <c r="R13" s="1">
+        <f>Q13*0.8</f>
+        <v>820</v>
+      </c>
+      <c r="S13" s="1">
+        <f>Q13*1.2</f>
+        <v>1230</v>
+      </c>
+      <c r="T13" s="1">
+        <v>1025</v>
+      </c>
+      <c r="U13" s="1">
+        <f>T13*0.8</f>
+        <v>820</v>
+      </c>
+      <c r="V13" s="1">
+        <f>T13*1.2</f>
+        <v>1230</v>
+      </c>
+      <c r="W13" s="1">
+        <v>1025</v>
+      </c>
+      <c r="X13" s="1">
+        <f>W13*0.8</f>
+        <v>820</v>
+      </c>
+      <c r="Y13" s="1">
+        <f>W13*1.2</f>
+        <v>1230</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>1025</v>
+      </c>
+      <c r="AA13" s="1">
+        <f>Z13*0.8</f>
+        <v>820</v>
+      </c>
+      <c r="AB13" s="1">
+        <f>Z13*1.2</f>
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="1">
+        <v>600</v>
+      </c>
+      <c r="L14" s="1">
+        <f>K14*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="M14" s="1">
+        <f>K14*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="N14" s="1">
+        <v>600</v>
+      </c>
+      <c r="O14" s="1">
+        <f>N14*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="P14" s="1">
+        <f>N14*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>600</v>
+      </c>
+      <c r="R14" s="1">
+        <f>Q14*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="S14" s="1">
+        <f>Q14*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="T14" s="1">
+        <v>600</v>
+      </c>
+      <c r="U14" s="1">
+        <f>T14*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="V14" s="1">
+        <f>T14*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="W14" s="1">
+        <v>600</v>
+      </c>
+      <c r="X14" s="1">
+        <f>W14*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="Y14" s="1">
+        <f>W14*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>600</v>
+      </c>
+      <c r="AA14" s="1">
+        <f>Z14*0.8</f>
+        <v>480</v>
+      </c>
+      <c r="AB14" s="1">
+        <f>Z14*1.2</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="1">
         <f>1100+8050</f>
         <v>9150</v>
       </c>
-      <c r="L12" s="1">
-        <f>K12*0.8</f>
+      <c r="L15" s="1">
+        <f>K15*0.8</f>
         <v>7320</v>
       </c>
-      <c r="M12" s="1">
-        <f>K12*1.2</f>
+      <c r="M15" s="1">
+        <f>K15*1.2</f>
         <v>10980</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N15" s="1">
         <f>1100+8050</f>
         <v>9150</v>
       </c>
-      <c r="O12" s="1">
-        <f>N12*0.8</f>
+      <c r="O15" s="1">
+        <f>N15*0.8</f>
         <v>7320</v>
       </c>
-      <c r="P12" s="1">
-        <f>N12*1.2</f>
+      <c r="P15" s="1">
+        <f>N15*1.2</f>
         <v>10980</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="Q15" s="1">
         <f>1100+8050</f>
         <v>9150</v>
       </c>
-      <c r="R12" s="1">
-        <f>Q12*0.8</f>
+      <c r="R15" s="1">
+        <f>Q15*0.8</f>
         <v>7320</v>
       </c>
-      <c r="S12" s="1">
-        <f>Q12*1.2</f>
+      <c r="S15" s="1">
+        <f>Q15*1.2</f>
         <v>10980</v>
       </c>
-      <c r="T12" s="1">
+      <c r="T15" s="1">
         <f>1100+8050</f>
         <v>9150</v>
       </c>
-      <c r="U12" s="1">
-        <f>T12*0.8</f>
+      <c r="U15" s="1">
+        <f>T15*0.8</f>
         <v>7320</v>
       </c>
-      <c r="V12" s="1">
-        <f>T12*1.2</f>
+      <c r="V15" s="1">
+        <f>T15*1.2</f>
         <v>10980</v>
       </c>
-      <c r="W12" s="1">
+      <c r="W15" s="1">
         <f>1100+8050</f>
         <v>9150</v>
       </c>
-      <c r="X12" s="1">
-        <f>W12*0.8</f>
+      <c r="X15" s="1">
+        <f>W15*0.8</f>
         <v>7320</v>
       </c>
-      <c r="Y12" s="1">
-        <f>W12*1.2</f>
+      <c r="Y15" s="1">
+        <f>W15*1.2</f>
         <v>10980</v>
       </c>
-      <c r="Z12" s="1">
+      <c r="Z15" s="1">
         <f>1100+8050</f>
         <v>9150</v>
       </c>
-      <c r="AA12" s="1">
-        <f>Z12*0.8</f>
+      <c r="AA15" s="1">
+        <f>Z15*0.8</f>
         <v>7320</v>
       </c>
-      <c r="AB12" s="1">
-        <f>Z12*1.2</f>
+      <c r="AB15" s="1">
+        <f>Z15*1.2</f>
         <v>10980</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K13" s="1">
-        <v>50</v>
-      </c>
-      <c r="L13" s="1">
-        <f t="shared" ref="L13:L30" si="0">K13*0.8</f>
-        <v>40</v>
-      </c>
-      <c r="M13" s="1">
-        <f t="shared" ref="M13" si="1">K13*1.2</f>
-        <v>60</v>
-      </c>
-      <c r="N13" s="1">
-        <v>50</v>
-      </c>
-      <c r="O13" s="1">
-        <f t="shared" ref="O13:O30" si="2">N13*0.8</f>
-        <v>40</v>
-      </c>
-      <c r="P13" s="1">
-        <f t="shared" ref="P13" si="3">N13*1.2</f>
-        <v>60</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>50</v>
-      </c>
-      <c r="R13" s="1">
-        <f t="shared" ref="R13:R30" si="4">Q13*0.8</f>
-        <v>40</v>
-      </c>
-      <c r="S13" s="1">
-        <f t="shared" ref="S13" si="5">Q13*1.2</f>
-        <v>60</v>
-      </c>
-      <c r="T13" s="1">
-        <v>50</v>
-      </c>
-      <c r="U13" s="1">
-        <f t="shared" ref="U13:U30" si="6">T13*0.8</f>
-        <v>40</v>
-      </c>
-      <c r="V13" s="1">
-        <f t="shared" ref="V13:V30" si="7">T13*1.2</f>
-        <v>60</v>
-      </c>
-      <c r="W13" s="1">
-        <v>50</v>
-      </c>
-      <c r="X13" s="1">
-        <f t="shared" ref="X13:X30" si="8">W13*0.8</f>
-        <v>40</v>
-      </c>
-      <c r="Y13" s="1">
-        <f t="shared" ref="Y13" si="9">W13*1.2</f>
-        <v>60</v>
-      </c>
-      <c r="Z13" s="1">
-        <v>50</v>
-      </c>
-      <c r="AA13" s="1">
-        <f t="shared" ref="AA13:AA30" si="10">Z13*0.8</f>
-        <v>40</v>
-      </c>
-      <c r="AB13" s="1">
-        <f t="shared" ref="AB13" si="11">Z13*1.2</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="1">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>0</v>
-      </c>
-      <c r="T14" s="1">
-        <v>0</v>
-      </c>
-      <c r="W14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0</v>
-      </c>
-      <c r="N15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>0</v>
-      </c>
-      <c r="T15" s="1">
-        <v>0</v>
-      </c>
-      <c r="W15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1813,10 +1760,10 @@
         <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>23</v>
@@ -1824,33 +1771,80 @@
       <c r="G16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="1" t="s">
-        <v>33</v>
+      <c r="H16" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="K16" s="1">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" ref="L16:L33" si="0">K16*0.8</f>
+        <v>40</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" ref="M16" si="1">K16*1.2</f>
+        <v>60</v>
       </c>
       <c r="N16" s="1">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" ref="O16:O33" si="2">N16*0.8</f>
+        <v>40</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" ref="P16" si="3">N16*1.2</f>
+        <v>60</v>
       </c>
       <c r="Q16" s="1">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="R16" s="1">
+        <f t="shared" ref="R16:R33" si="4">Q16*0.8</f>
+        <v>40</v>
+      </c>
+      <c r="S16" s="1">
+        <f t="shared" ref="S16" si="5">Q16*1.2</f>
+        <v>60</v>
       </c>
       <c r="T16" s="1">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="U16" s="1">
+        <f t="shared" ref="U16:U33" si="6">T16*0.8</f>
+        <v>40</v>
+      </c>
+      <c r="V16" s="1">
+        <f t="shared" ref="V16:V33" si="7">T16*1.2</f>
+        <v>60</v>
       </c>
       <c r="W16" s="1">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="X16" s="1">
+        <f t="shared" ref="X16:X33" si="8">W16*0.8</f>
+        <v>40</v>
+      </c>
+      <c r="Y16" s="1">
+        <f t="shared" ref="Y16" si="9">W16*1.2</f>
+        <v>60</v>
       </c>
       <c r="Z16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="AA16" s="1">
+        <f t="shared" ref="AA16:AA33" si="10">Z16*0.8</f>
+        <v>40</v>
+      </c>
+      <c r="AB16" s="1">
+        <f t="shared" ref="AB16" si="11">Z16*1.2</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1861,7 +1855,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>29</v>
@@ -1880,25 +1874,25 @@
         <v>10</v>
       </c>
       <c r="K17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1909,7 +1903,7 @@
         <v>19</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>29</v>
@@ -1946,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1957,7 +1951,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>29</v>
@@ -1994,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -2005,7 +1999,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>29</v>
@@ -2042,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -2053,7 +2047,7 @@
         <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>29</v>
@@ -2090,7 +2084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -2101,7 +2095,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>29</v>
@@ -2138,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -2149,7 +2143,7 @@
         <v>19</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>29</v>
@@ -2186,7 +2180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -2197,7 +2191,7 @@
         <v>19</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>29</v>
@@ -2216,25 +2210,25 @@
         <v>10</v>
       </c>
       <c r="K24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -2245,7 +2239,7 @@
         <v>19</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>29</v>
@@ -2264,25 +2258,25 @@
         <v>10</v>
       </c>
       <c r="K25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -2293,7 +2287,7 @@
         <v>19</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>29</v>
@@ -2312,39 +2306,39 @@
         <v>10</v>
       </c>
       <c r="K26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z26" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>23</v>
@@ -2352,526 +2346,526 @@
       <c r="G27" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H27" s="5"/>
       <c r="I27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>1</v>
+      </c>
+      <c r="T27" s="1">
+        <v>1</v>
+      </c>
+      <c r="W27" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="5"/>
+      <c r="I28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>0</v>
+      </c>
+      <c r="T28" s="1">
+        <v>0</v>
+      </c>
+      <c r="W28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0</v>
+      </c>
+      <c r="T29" s="1">
+        <v>0</v>
+      </c>
+      <c r="W29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K30" s="1">
         <v>50</v>
       </c>
-      <c r="L27" s="1">
+      <c r="L30" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="M27" s="1">
-        <f t="shared" ref="M27" si="12">K27*1.2</f>
+      <c r="M30" s="1">
+        <f t="shared" ref="M30" si="12">K30*1.2</f>
         <v>60</v>
       </c>
-      <c r="N27" s="1">
+      <c r="N30" s="1">
         <v>50</v>
       </c>
-      <c r="O27" s="1">
+      <c r="O30" s="1">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="P27" s="1">
-        <f t="shared" ref="P27" si="13">N27*1.2</f>
+      <c r="P30" s="1">
+        <f t="shared" ref="P30" si="13">N30*1.2</f>
         <v>60</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="Q30" s="1">
         <v>50</v>
       </c>
-      <c r="R27" s="1">
+      <c r="R30" s="1">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="S27" s="1">
-        <f t="shared" ref="S27" si="14">Q27*1.2</f>
+      <c r="S30" s="1">
+        <f t="shared" ref="S30" si="14">Q30*1.2</f>
         <v>60</v>
       </c>
-      <c r="T27" s="1">
+      <c r="T30" s="1">
         <v>50</v>
       </c>
-      <c r="U27" s="1">
+      <c r="U30" s="1">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="V27" s="1">
+      <c r="V30" s="1">
         <f t="shared" si="7"/>
         <v>60</v>
       </c>
-      <c r="W27" s="1">
+      <c r="W30" s="1">
         <v>50</v>
       </c>
-      <c r="X27" s="1">
+      <c r="X30" s="1">
         <f t="shared" si="8"/>
         <v>40</v>
       </c>
-      <c r="Y27" s="1">
-        <f t="shared" ref="Y27" si="15">W27*1.2</f>
+      <c r="Y30" s="1">
+        <f t="shared" ref="Y30" si="15">W30*1.2</f>
         <v>60</v>
       </c>
-      <c r="Z27" s="1">
+      <c r="Z30" s="1">
         <v>50</v>
       </c>
-      <c r="AA27" s="1">
+      <c r="AA30" s="1">
         <f t="shared" si="10"/>
         <v>40</v>
       </c>
-      <c r="AB27" s="1">
-        <f t="shared" ref="AB27" si="16">Z27*1.2</f>
+      <c r="AB30" s="1">
+        <f t="shared" ref="AB30" si="16">Z30*1.2</f>
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="C31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I28" s="1" t="s">
+      <c r="G31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K31" s="1">
         <v>50</v>
       </c>
-      <c r="L28" s="1">
+      <c r="L31" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="M28" s="1">
-        <f t="shared" ref="M28:M29" si="17">K28*1.2</f>
+      <c r="M31" s="1">
+        <f t="shared" ref="M31:M32" si="17">K31*1.2</f>
         <v>60</v>
       </c>
-      <c r="N28" s="1">
+      <c r="N31" s="1">
         <v>50</v>
       </c>
-      <c r="O28" s="1">
+      <c r="O31" s="1">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="P28" s="1">
-        <f t="shared" ref="P28:P29" si="18">N28*1.2</f>
+      <c r="P31" s="1">
+        <f t="shared" ref="P31:P32" si="18">N31*1.2</f>
         <v>60</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="Q31" s="1">
         <v>50</v>
       </c>
-      <c r="R28" s="1">
+      <c r="R31" s="1">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="S28" s="1">
-        <f t="shared" ref="S28:S29" si="19">Q28*1.2</f>
+      <c r="S31" s="1">
+        <f t="shared" ref="S31:S32" si="19">Q31*1.2</f>
         <v>60</v>
       </c>
-      <c r="T28" s="1">
+      <c r="T31" s="1">
         <v>50</v>
       </c>
-      <c r="U28" s="1">
+      <c r="U31" s="1">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="V28" s="1">
+      <c r="V31" s="1">
         <f t="shared" si="7"/>
         <v>60</v>
       </c>
-      <c r="W28" s="1">
+      <c r="W31" s="1">
         <v>50</v>
       </c>
-      <c r="X28" s="1">
+      <c r="X31" s="1">
         <f t="shared" si="8"/>
         <v>40</v>
       </c>
-      <c r="Y28" s="1">
-        <f t="shared" ref="Y28:Y29" si="20">W28*1.2</f>
+      <c r="Y31" s="1">
+        <f t="shared" ref="Y31:Y32" si="20">W31*1.2</f>
         <v>60</v>
       </c>
-      <c r="Z28" s="1">
+      <c r="Z31" s="1">
         <v>50</v>
       </c>
-      <c r="AA28" s="1">
+      <c r="AA31" s="1">
         <f t="shared" si="10"/>
         <v>40</v>
       </c>
-      <c r="AB28" s="1">
-        <f t="shared" ref="AB28:AB29" si="21">Z28*1.2</f>
+      <c r="AB31" s="1">
+        <f t="shared" ref="AB31:AB32" si="21">Z31*1.2</f>
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H29" s="5" t="s">
+      <c r="G32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K32" s="1">
         <f>2160/30</f>
         <v>72</v>
       </c>
-      <c r="L29" s="1">
+      <c r="L32" s="1">
         <f t="shared" si="0"/>
         <v>57.6</v>
       </c>
-      <c r="M29" s="1">
+      <c r="M32" s="1">
         <f t="shared" si="17"/>
         <v>86.399999999999991</v>
       </c>
-      <c r="N29" s="1">
+      <c r="N32" s="1">
         <f>2160/30</f>
         <v>72</v>
       </c>
-      <c r="O29" s="1">
+      <c r="O32" s="1">
         <f t="shared" si="2"/>
         <v>57.6</v>
       </c>
-      <c r="P29" s="1">
+      <c r="P32" s="1">
         <f t="shared" si="18"/>
         <v>86.399999999999991</v>
       </c>
-      <c r="Q29" s="1">
+      <c r="Q32" s="1">
         <f>2160/30</f>
         <v>72</v>
       </c>
-      <c r="R29" s="1">
+      <c r="R32" s="1">
         <f t="shared" si="4"/>
         <v>57.6</v>
       </c>
-      <c r="S29" s="1">
+      <c r="S32" s="1">
         <f t="shared" si="19"/>
         <v>86.399999999999991</v>
       </c>
-      <c r="T29" s="1">
+      <c r="T32" s="1">
         <f>2160/30</f>
         <v>72</v>
       </c>
-      <c r="U29" s="1">
+      <c r="U32" s="1">
         <f t="shared" si="6"/>
         <v>57.6</v>
       </c>
-      <c r="V29" s="1">
+      <c r="V32" s="1">
         <f t="shared" si="7"/>
         <v>86.399999999999991</v>
       </c>
-      <c r="W29" s="1">
+      <c r="W32" s="1">
         <f>2160/30</f>
         <v>72</v>
       </c>
-      <c r="X29" s="1">
+      <c r="X32" s="1">
         <f t="shared" si="8"/>
         <v>57.6</v>
       </c>
-      <c r="Y29" s="1">
+      <c r="Y32" s="1">
         <f t="shared" si="20"/>
         <v>86.399999999999991</v>
       </c>
-      <c r="Z29" s="1">
+      <c r="Z32" s="1">
         <f>2160/30</f>
         <v>72</v>
       </c>
-      <c r="AA29" s="1">
+      <c r="AA32" s="1">
         <f t="shared" si="10"/>
         <v>57.6</v>
       </c>
-      <c r="AB29" s="1">
+      <c r="AB32" s="1">
         <f t="shared" si="21"/>
         <v>86.399999999999991</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" s="5" t="s">
+      <c r="G33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K33" s="1">
         <v>600</v>
       </c>
-      <c r="L30" s="1">
+      <c r="L33" s="1">
         <f t="shared" si="0"/>
         <v>480</v>
       </c>
-      <c r="M30" s="1">
-        <f t="shared" ref="M30" si="22">K30*1.2</f>
+      <c r="M33" s="1">
+        <f t="shared" ref="M33" si="22">K33*1.2</f>
         <v>720</v>
       </c>
-      <c r="N30" s="1">
+      <c r="N33" s="1">
         <v>2160</v>
       </c>
-      <c r="O30" s="1">
+      <c r="O33" s="1">
         <f t="shared" si="2"/>
         <v>1728</v>
       </c>
-      <c r="P30" s="1">
-        <f t="shared" ref="P30" si="23">N30*1.2</f>
+      <c r="P33" s="1">
+        <f t="shared" ref="P33" si="23">N33*1.2</f>
         <v>2592</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="Q33" s="1">
         <v>2160</v>
       </c>
-      <c r="R30" s="1">
+      <c r="R33" s="1">
         <f t="shared" si="4"/>
         <v>1728</v>
       </c>
-      <c r="S30" s="1">
-        <f t="shared" ref="S30" si="24">Q30*1.2</f>
+      <c r="S33" s="1">
+        <f t="shared" ref="S33" si="24">Q33*1.2</f>
         <v>2592</v>
       </c>
-      <c r="T30" s="1">
+      <c r="T33" s="1">
         <v>2160</v>
       </c>
-      <c r="U30" s="1">
+      <c r="U33" s="1">
         <f t="shared" si="6"/>
         <v>1728</v>
       </c>
-      <c r="V30" s="1">
+      <c r="V33" s="1">
         <f t="shared" si="7"/>
         <v>2592</v>
       </c>
-      <c r="W30" s="1">
+      <c r="W33" s="1">
         <v>2160</v>
       </c>
-      <c r="X30" s="1">
+      <c r="X33" s="1">
         <f t="shared" si="8"/>
         <v>1728</v>
       </c>
-      <c r="Y30" s="1">
-        <f t="shared" ref="Y30" si="25">W30*1.2</f>
+      <c r="Y33" s="1">
+        <f t="shared" ref="Y33" si="25">W33*1.2</f>
         <v>2592</v>
       </c>
-      <c r="Z30" s="1">
+      <c r="Z33" s="1">
         <v>2160</v>
       </c>
-      <c r="AA30" s="1">
+      <c r="AA33" s="1">
         <f t="shared" si="10"/>
         <v>1728</v>
       </c>
-      <c r="AB30" s="1">
-        <f t="shared" ref="AB30" si="26">Z30*1.2</f>
+      <c r="AB33" s="1">
+        <f t="shared" ref="AB33" si="26">Z33*1.2</f>
         <v>2592</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K31" s="1">
-        <v>0</v>
-      </c>
-      <c r="N31" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="1">
-        <v>0</v>
-      </c>
-      <c r="T31" s="1">
-        <v>0</v>
-      </c>
-      <c r="W31" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32" s="5"/>
-      <c r="I32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K32" s="1">
-        <v>0</v>
-      </c>
-      <c r="N32" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="1">
-        <v>0</v>
-      </c>
-      <c r="T32" s="1">
-        <v>0</v>
-      </c>
-      <c r="W32" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H33" s="5"/>
-      <c r="I33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K33" s="1">
-        <v>0</v>
-      </c>
-      <c r="N33" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="1">
-        <v>0</v>
-      </c>
-      <c r="T33" s="1">
-        <v>0</v>
-      </c>
-      <c r="W33" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>29</v>
@@ -2890,39 +2884,39 @@
         <v>10</v>
       </c>
       <c r="K34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>23</v>
@@ -2930,82 +2924,35 @@
       <c r="G35" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H35" s="5"/>
       <c r="I35" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="K35" s="1">
-        <v>2400</v>
-      </c>
-      <c r="L35" s="1">
-        <f t="shared" ref="L35:L43" si="27">K35*0.9</f>
-        <v>2160</v>
-      </c>
-      <c r="M35" s="1">
-        <f t="shared" ref="M35:M43" si="28">K35*1.1</f>
-        <v>2640</v>
+        <v>0</v>
       </c>
       <c r="N35" s="1">
-        <v>2400</v>
-      </c>
-      <c r="O35" s="1">
-        <f t="shared" ref="O35:O43" si="29">N35*0.9</f>
-        <v>2160</v>
-      </c>
-      <c r="P35" s="1">
-        <f t="shared" ref="P35:P43" si="30">N35*1.1</f>
-        <v>2640</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="1">
-        <v>2400</v>
-      </c>
-      <c r="R35" s="1">
-        <f t="shared" ref="R35:R43" si="31">Q35*0.9</f>
-        <v>2160</v>
-      </c>
-      <c r="S35" s="1">
-        <f t="shared" ref="S35:S43" si="32">Q35*1.1</f>
-        <v>2640</v>
+        <v>0</v>
       </c>
       <c r="T35" s="1">
-        <v>2400</v>
-      </c>
-      <c r="U35" s="1">
-        <f t="shared" ref="U35:U42" si="33">T35*0.9</f>
-        <v>2160</v>
-      </c>
-      <c r="V35" s="1">
-        <f t="shared" ref="V35:V42" si="34">T35*1.1</f>
-        <v>2640</v>
+        <v>0</v>
       </c>
       <c r="W35" s="1">
-        <v>2400</v>
-      </c>
-      <c r="X35" s="1">
-        <f t="shared" ref="X35:X43" si="35">W35*0.9</f>
-        <v>2160</v>
-      </c>
-      <c r="Y35" s="1">
-        <f t="shared" ref="Y35:Y43" si="36">W35*1.1</f>
-        <v>2640</v>
+        <v>0</v>
       </c>
       <c r="Z35" s="1">
-        <v>2400</v>
-      </c>
-      <c r="AA35" s="1">
-        <f t="shared" ref="AA35:AA43" si="37">Z35*0.9</f>
-        <v>2160</v>
-      </c>
-      <c r="AB35" s="1">
-        <f t="shared" ref="AB35:AB43" si="38">Z35*1.1</f>
-        <v>2640</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>20</v>
@@ -3014,10 +2961,10 @@
         <v>19</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>23</v>
@@ -3025,692 +2972,883 @@
       <c r="G36" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H36" s="5"/>
       <c r="I36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>0</v>
+      </c>
+      <c r="T36" s="1">
+        <v>0</v>
+      </c>
+      <c r="W36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="5"/>
+      <c r="I37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K37" s="1">
+        <v>1</v>
+      </c>
+      <c r="N37" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>1</v>
+      </c>
+      <c r="T37" s="1">
+        <v>1</v>
+      </c>
+      <c r="W37" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K38" s="1">
+        <v>2400</v>
+      </c>
+      <c r="L38" s="1">
+        <f t="shared" ref="L38:L45" si="27">K38*0.9</f>
+        <v>2160</v>
+      </c>
+      <c r="M38" s="1">
+        <f t="shared" ref="M38:M45" si="28">K38*1.1</f>
+        <v>2640</v>
+      </c>
+      <c r="N38" s="1">
+        <v>2400</v>
+      </c>
+      <c r="O38" s="1">
+        <f t="shared" ref="O38:O45" si="29">N38*0.9</f>
+        <v>2160</v>
+      </c>
+      <c r="P38" s="1">
+        <f t="shared" ref="P38:P45" si="30">N38*1.1</f>
+        <v>2640</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>2400</v>
+      </c>
+      <c r="R38" s="1">
+        <f t="shared" ref="R38:R45" si="31">Q38*0.9</f>
+        <v>2160</v>
+      </c>
+      <c r="S38" s="1">
+        <f t="shared" ref="S38:S45" si="32">Q38*1.1</f>
+        <v>2640</v>
+      </c>
+      <c r="T38" s="1">
+        <v>2400</v>
+      </c>
+      <c r="U38" s="1">
+        <f t="shared" ref="U38:U45" si="33">T38*0.9</f>
+        <v>2160</v>
+      </c>
+      <c r="V38" s="1">
+        <f t="shared" ref="V38:V45" si="34">T38*1.1</f>
+        <v>2640</v>
+      </c>
+      <c r="W38" s="1">
+        <v>2400</v>
+      </c>
+      <c r="X38" s="1">
+        <f t="shared" ref="X38:X45" si="35">W38*0.9</f>
+        <v>2160</v>
+      </c>
+      <c r="Y38" s="1">
+        <f t="shared" ref="Y38:Y45" si="36">W38*1.1</f>
+        <v>2640</v>
+      </c>
+      <c r="Z38" s="1">
+        <v>2400</v>
+      </c>
+      <c r="AA38" s="1">
+        <f t="shared" ref="AA38:AA45" si="37">Z38*0.9</f>
+        <v>2160</v>
+      </c>
+      <c r="AB38" s="1">
+        <f t="shared" ref="AB38:AB45" si="38">Z38*1.1</f>
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K39" s="1">
         <v>300</v>
       </c>
-      <c r="L36" s="1">
+      <c r="L39" s="1">
         <f t="shared" si="27"/>
         <v>270</v>
       </c>
-      <c r="M36" s="1">
+      <c r="M39" s="1">
         <f t="shared" si="28"/>
         <v>330</v>
       </c>
-      <c r="N36" s="1">
+      <c r="N39" s="1">
         <v>300</v>
       </c>
-      <c r="O36" s="1">
+      <c r="O39" s="1">
         <f t="shared" si="29"/>
         <v>270</v>
       </c>
-      <c r="P36" s="1">
+      <c r="P39" s="1">
         <f t="shared" si="30"/>
         <v>330</v>
       </c>
-      <c r="Q36" s="1">
+      <c r="Q39" s="1">
         <v>300</v>
       </c>
-      <c r="R36" s="1">
+      <c r="R39" s="1">
         <f t="shared" si="31"/>
         <v>270</v>
       </c>
-      <c r="S36" s="1">
+      <c r="S39" s="1">
         <f t="shared" si="32"/>
         <v>330</v>
       </c>
-      <c r="T36" s="1">
+      <c r="T39" s="1">
         <v>300</v>
       </c>
-      <c r="U36" s="1">
+      <c r="U39" s="1">
         <f t="shared" si="33"/>
         <v>270</v>
       </c>
-      <c r="V36" s="1">
+      <c r="V39" s="1">
         <f t="shared" si="34"/>
         <v>330</v>
       </c>
-      <c r="W36" s="1">
+      <c r="W39" s="1">
         <v>300</v>
       </c>
-      <c r="X36" s="1">
+      <c r="X39" s="1">
         <f t="shared" si="35"/>
         <v>270</v>
       </c>
-      <c r="Y36" s="1">
+      <c r="Y39" s="1">
         <f t="shared" si="36"/>
         <v>330</v>
       </c>
-      <c r="Z36" s="1">
+      <c r="Z39" s="1">
         <v>300</v>
       </c>
-      <c r="AA36" s="1">
+      <c r="AA39" s="1">
         <f t="shared" si="37"/>
         <v>270</v>
       </c>
-      <c r="AB36" s="1">
+      <c r="AB39" s="1">
         <f t="shared" si="38"/>
         <v>330</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="C40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="1" t="s">
+      <c r="G40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K40" s="1">
         <v>300</v>
       </c>
-      <c r="L37" s="1">
+      <c r="L40" s="1">
         <f t="shared" si="27"/>
         <v>270</v>
       </c>
-      <c r="M37" s="1">
+      <c r="M40" s="1">
         <f t="shared" si="28"/>
         <v>330</v>
       </c>
-      <c r="N37" s="1">
+      <c r="N40" s="1">
         <v>300</v>
       </c>
-      <c r="O37" s="1">
+      <c r="O40" s="1">
         <f t="shared" si="29"/>
         <v>270</v>
       </c>
-      <c r="P37" s="1">
+      <c r="P40" s="1">
         <f t="shared" si="30"/>
         <v>330</v>
       </c>
-      <c r="Q37" s="1">
+      <c r="Q40" s="1">
         <v>300</v>
       </c>
-      <c r="R37" s="1">
+      <c r="R40" s="1">
         <f t="shared" si="31"/>
         <v>270</v>
       </c>
-      <c r="S37" s="1">
+      <c r="S40" s="1">
         <f t="shared" si="32"/>
         <v>330</v>
       </c>
-      <c r="T37" s="1">
+      <c r="T40" s="1">
         <v>300</v>
       </c>
-      <c r="U37" s="1">
+      <c r="U40" s="1">
         <f t="shared" si="33"/>
         <v>270</v>
       </c>
-      <c r="V37" s="1">
+      <c r="V40" s="1">
         <f t="shared" si="34"/>
         <v>330</v>
       </c>
-      <c r="W37" s="1">
+      <c r="W40" s="1">
         <v>300</v>
       </c>
-      <c r="X37" s="1">
+      <c r="X40" s="1">
         <f t="shared" si="35"/>
         <v>270</v>
       </c>
-      <c r="Y37" s="1">
+      <c r="Y40" s="1">
         <f t="shared" si="36"/>
         <v>330</v>
       </c>
-      <c r="Z37" s="1">
+      <c r="Z40" s="1">
         <v>300</v>
       </c>
-      <c r="AA37" s="1">
+      <c r="AA40" s="1">
         <f t="shared" si="37"/>
         <v>270</v>
       </c>
-      <c r="AB37" s="1">
+      <c r="AB40" s="1">
         <f t="shared" si="38"/>
         <v>330</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="C41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K41" s="1">
         <v>20</v>
       </c>
-      <c r="L38" s="1">
+      <c r="L41" s="1">
         <f t="shared" si="27"/>
         <v>18</v>
       </c>
-      <c r="M38" s="1">
+      <c r="M41" s="1">
         <f t="shared" si="28"/>
         <v>22</v>
       </c>
-      <c r="N38" s="1">
+      <c r="N41" s="1">
         <v>20</v>
       </c>
-      <c r="O38" s="1">
+      <c r="O41" s="1">
         <f t="shared" si="29"/>
         <v>18</v>
       </c>
-      <c r="P38" s="1">
+      <c r="P41" s="1">
         <f t="shared" si="30"/>
         <v>22</v>
       </c>
-      <c r="Q38" s="1">
+      <c r="Q41" s="1">
         <v>20</v>
       </c>
-      <c r="R38" s="1">
+      <c r="R41" s="1">
         <f t="shared" si="31"/>
         <v>18</v>
       </c>
-      <c r="S38" s="1">
+      <c r="S41" s="1">
         <f t="shared" si="32"/>
         <v>22</v>
       </c>
-      <c r="T38" s="1">
+      <c r="T41" s="1">
         <v>20</v>
       </c>
-      <c r="U38" s="1">
+      <c r="U41" s="1">
         <f t="shared" si="33"/>
         <v>18</v>
       </c>
-      <c r="V38" s="1">
+      <c r="V41" s="1">
         <f t="shared" si="34"/>
         <v>22</v>
       </c>
-      <c r="W38" s="1">
+      <c r="W41" s="1">
         <v>20</v>
       </c>
-      <c r="X38" s="1">
+      <c r="X41" s="1">
         <f t="shared" si="35"/>
         <v>18</v>
       </c>
-      <c r="Y38" s="1">
+      <c r="Y41" s="1">
         <f t="shared" si="36"/>
         <v>22</v>
       </c>
-      <c r="Z38" s="1">
+      <c r="Z41" s="1">
         <v>20</v>
       </c>
-      <c r="AA38" s="1">
+      <c r="AA41" s="1">
         <f t="shared" si="37"/>
         <v>18</v>
       </c>
-      <c r="AB38" s="1">
+      <c r="AB41" s="1">
         <f t="shared" si="38"/>
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="C42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K39" s="1">
+      <c r="K42" s="1">
         <v>25</v>
       </c>
-      <c r="L39" s="1">
+      <c r="L42" s="1">
         <f t="shared" si="27"/>
         <v>22.5</v>
       </c>
-      <c r="M39" s="1">
+      <c r="M42" s="1">
         <f t="shared" si="28"/>
         <v>27.500000000000004</v>
       </c>
-      <c r="N39" s="1">
+      <c r="N42" s="1">
         <v>25</v>
       </c>
-      <c r="O39" s="1">
+      <c r="O42" s="1">
         <f t="shared" si="29"/>
         <v>22.5</v>
       </c>
-      <c r="P39" s="1">
+      <c r="P42" s="1">
         <f t="shared" si="30"/>
         <v>27.500000000000004</v>
       </c>
-      <c r="Q39" s="1">
+      <c r="Q42" s="1">
         <v>25</v>
       </c>
-      <c r="R39" s="1">
+      <c r="R42" s="1">
         <f t="shared" si="31"/>
         <v>22.5</v>
       </c>
-      <c r="S39" s="1">
+      <c r="S42" s="1">
         <f t="shared" si="32"/>
         <v>27.500000000000004</v>
       </c>
-      <c r="T39" s="1">
+      <c r="T42" s="1">
         <v>25</v>
       </c>
-      <c r="U39" s="1">
+      <c r="U42" s="1">
         <f t="shared" si="33"/>
         <v>22.5</v>
       </c>
-      <c r="V39" s="1">
+      <c r="V42" s="1">
         <f t="shared" si="34"/>
         <v>27.500000000000004</v>
       </c>
-      <c r="W39" s="1">
+      <c r="W42" s="1">
         <v>25</v>
       </c>
-      <c r="X39" s="1">
+      <c r="X42" s="1">
         <f t="shared" si="35"/>
         <v>22.5</v>
       </c>
-      <c r="Y39" s="1">
+      <c r="Y42" s="1">
         <f t="shared" si="36"/>
         <v>27.500000000000004</v>
       </c>
-      <c r="Z39" s="1">
+      <c r="Z42" s="1">
         <v>25</v>
       </c>
-      <c r="AA39" s="1">
+      <c r="AA42" s="1">
         <f t="shared" si="37"/>
         <v>22.5</v>
       </c>
-      <c r="AB39" s="1">
+      <c r="AB42" s="1">
         <f t="shared" si="38"/>
         <v>27.500000000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="C43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K43" s="1">
         <v>5</v>
       </c>
-      <c r="L40" s="1">
+      <c r="L43" s="1">
         <f t="shared" si="27"/>
         <v>4.5</v>
       </c>
-      <c r="M40" s="1">
+      <c r="M43" s="1">
         <f t="shared" si="28"/>
         <v>5.5</v>
       </c>
-      <c r="N40" s="1">
+      <c r="N43" s="1">
         <v>5</v>
       </c>
-      <c r="O40" s="1">
+      <c r="O43" s="1">
         <f t="shared" si="29"/>
         <v>4.5</v>
       </c>
-      <c r="P40" s="1">
+      <c r="P43" s="1">
         <f t="shared" si="30"/>
         <v>5.5</v>
       </c>
-      <c r="Q40" s="1">
+      <c r="Q43" s="1">
         <v>5</v>
       </c>
-      <c r="R40" s="1">
+      <c r="R43" s="1">
         <f t="shared" si="31"/>
         <v>4.5</v>
       </c>
-      <c r="S40" s="1">
+      <c r="S43" s="1">
         <f t="shared" si="32"/>
         <v>5.5</v>
       </c>
-      <c r="T40" s="1">
+      <c r="T43" s="1">
         <v>5</v>
       </c>
-      <c r="U40" s="1">
+      <c r="U43" s="1">
         <f t="shared" si="33"/>
         <v>4.5</v>
       </c>
-      <c r="V40" s="1">
+      <c r="V43" s="1">
         <f t="shared" si="34"/>
         <v>5.5</v>
       </c>
-      <c r="W40" s="1">
+      <c r="W43" s="1">
         <v>5</v>
       </c>
-      <c r="X40" s="1">
+      <c r="X43" s="1">
         <f t="shared" si="35"/>
         <v>4.5</v>
       </c>
-      <c r="Y40" s="1">
+      <c r="Y43" s="1">
         <f t="shared" si="36"/>
         <v>5.5</v>
       </c>
-      <c r="Z40" s="1">
+      <c r="Z43" s="1">
         <v>5</v>
       </c>
-      <c r="AA40" s="1">
+      <c r="AA43" s="1">
         <f t="shared" si="37"/>
         <v>4.5</v>
       </c>
-      <c r="AB40" s="1">
+      <c r="AB43" s="1">
         <f t="shared" si="38"/>
         <v>5.5</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K44" s="1">
         <v>50</v>
       </c>
-      <c r="L41" s="1">
+      <c r="L44" s="1">
         <f t="shared" si="27"/>
         <v>45</v>
       </c>
-      <c r="M41" s="1">
+      <c r="M44" s="1">
         <f t="shared" si="28"/>
         <v>55.000000000000007</v>
       </c>
-      <c r="N41" s="1">
+      <c r="N44" s="1">
         <v>50</v>
       </c>
-      <c r="O41" s="1">
+      <c r="O44" s="1">
         <f t="shared" si="29"/>
         <v>45</v>
       </c>
-      <c r="P41" s="1">
+      <c r="P44" s="1">
         <f t="shared" si="30"/>
         <v>55.000000000000007</v>
       </c>
-      <c r="Q41" s="1">
+      <c r="Q44" s="1">
         <v>50</v>
       </c>
-      <c r="R41" s="1">
+      <c r="R44" s="1">
         <f t="shared" si="31"/>
         <v>45</v>
       </c>
-      <c r="S41" s="1">
+      <c r="S44" s="1">
         <f t="shared" si="32"/>
         <v>55.000000000000007</v>
       </c>
-      <c r="T41" s="1">
+      <c r="T44" s="1">
         <v>50</v>
       </c>
-      <c r="U41" s="1">
+      <c r="U44" s="1">
         <f t="shared" si="33"/>
         <v>45</v>
       </c>
-      <c r="V41" s="1">
+      <c r="V44" s="1">
         <f t="shared" si="34"/>
         <v>55.000000000000007</v>
       </c>
-      <c r="W41" s="1">
+      <c r="W44" s="1">
         <v>50</v>
       </c>
-      <c r="X41" s="1">
+      <c r="X44" s="1">
         <f t="shared" si="35"/>
         <v>45</v>
       </c>
-      <c r="Y41" s="1">
+      <c r="Y44" s="1">
         <f t="shared" si="36"/>
         <v>55.000000000000007</v>
       </c>
-      <c r="Z41" s="1">
+      <c r="Z44" s="1">
         <v>50</v>
       </c>
-      <c r="AA41" s="1">
+      <c r="AA44" s="1">
         <f t="shared" si="37"/>
         <v>45</v>
       </c>
-      <c r="AB41" s="1">
+      <c r="AB44" s="1">
         <f t="shared" si="38"/>
         <v>55.000000000000007</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="C45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="J45" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K42" s="1">
+      <c r="K45" s="1">
         <v>500</v>
       </c>
-      <c r="L42" s="1">
+      <c r="L45" s="1">
         <f t="shared" si="27"/>
         <v>450</v>
       </c>
-      <c r="M42" s="1">
+      <c r="M45" s="1">
         <f t="shared" si="28"/>
         <v>550</v>
       </c>
-      <c r="N42" s="1">
+      <c r="N45" s="1">
         <v>500</v>
       </c>
-      <c r="O42" s="1">
+      <c r="O45" s="1">
         <f t="shared" si="29"/>
         <v>450</v>
       </c>
-      <c r="P42" s="1">
+      <c r="P45" s="1">
         <f t="shared" si="30"/>
         <v>550</v>
       </c>
-      <c r="Q42" s="1">
+      <c r="Q45" s="1">
         <v>500</v>
       </c>
-      <c r="R42" s="1">
+      <c r="R45" s="1">
         <f t="shared" si="31"/>
         <v>450</v>
       </c>
-      <c r="S42" s="1">
+      <c r="S45" s="1">
         <f t="shared" si="32"/>
         <v>550</v>
       </c>
-      <c r="T42" s="1">
+      <c r="T45" s="1">
         <v>500</v>
       </c>
-      <c r="U42" s="1">
+      <c r="U45" s="1">
         <f t="shared" si="33"/>
         <v>450</v>
       </c>
-      <c r="V42" s="1">
+      <c r="V45" s="1">
         <f t="shared" si="34"/>
         <v>550</v>
       </c>
-      <c r="W42" s="1">
+      <c r="W45" s="1">
         <v>500</v>
       </c>
-      <c r="X42" s="1">
+      <c r="X45" s="1">
         <f t="shared" si="35"/>
         <v>450</v>
       </c>
-      <c r="Y42" s="1">
+      <c r="Y45" s="1">
         <f t="shared" si="36"/>
         <v>550</v>
       </c>
-      <c r="Z42" s="1">
+      <c r="Z45" s="1">
         <v>500</v>
       </c>
-      <c r="AA42" s="1">
+      <c r="AA45" s="1">
         <f t="shared" si="37"/>
         <v>450</v>
       </c>
-      <c r="AB42" s="1">
+      <c r="AB45" s="1">
         <f t="shared" si="38"/>
         <v>550</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="C46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K43" s="1">
-        <v>1</v>
-      </c>
-      <c r="N43" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q43" s="1">
-        <v>1</v>
-      </c>
-      <c r="T43" s="1">
-        <v>1</v>
-      </c>
-      <c r="W43" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z43" s="1">
+      <c r="K46" s="1">
+        <v>1</v>
+      </c>
+      <c r="N46" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>1</v>
+      </c>
+      <c r="T46" s="1">
+        <v>1</v>
+      </c>
+      <c r="W46" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z46" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:Y42" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:Y45" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Made small modifications in the files update_input_params, turbines_input_params, model, wind_array for the code to run Added a part calculating the energy production per year, not finished yet.
</commit_message>
<xml_diff>
--- a/windisch/data/Input data.xlsx
+++ b/windisch/data/Input data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/windisch/windisch/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalenajonsson/Desktop/SemesterProject/Code/windisch_folder/windisch/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF7C247-53B1-6341-B13E-14D099B09B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BBAE2D-ED4A-AA42-AC3E-BE78081C43E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28420" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="73">
   <si>
     <t>parameter</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>power</t>
+  </si>
+  <si>
+    <t>unitless</t>
+  </si>
+  <si>
+    <t>average capacity factor</t>
   </si>
 </sst>
 </file>
@@ -317,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -334,9 +340,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -639,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB43"/>
+  <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="D23" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3660,6 +3669,106 @@
         <v>1</v>
       </c>
     </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K44" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="L44" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="M44" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="N44" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="O44" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="P44" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="Q44" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="R44" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="S44" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="T44" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="U44" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="V44" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="W44" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="X44" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="Y44" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="Z44" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="AA44" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="AB44" s="6">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:Y43" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Deleted cut_speeds.py calculated cut-in/cut-out wind speeds and stored them as default parameters. Code refactoring
</commit_message>
<xml_diff>
--- a/windisch/data/Input data.xlsx
+++ b/windisch/data/Input data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalenajonsson/Desktop/SemesterProject/Code/windisch_folder/windisch/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/windisch/windisch/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BBAE2D-ED4A-AA42-AC3E-BE78081C43E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1350EE9-4A54-CD4C-A438-10D63DD0C550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5140" yWindow="760" windowWidth="23280" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="77">
   <si>
     <t>parameter</t>
   </si>
@@ -253,14 +253,27 @@
   </si>
   <si>
     <t>average capacity factor</t>
+  </si>
+  <si>
+    <t>cut-in</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>Cut-in wind speed. Source: WindTurbine power curves database.</t>
+  </si>
+  <si>
+    <t>cut-out</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -323,7 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -343,9 +356,15 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -648,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB45"/>
+  <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D23" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3769,6 +3788,836 @@
         <v>56</v>
       </c>
     </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="8">
+        <v>100</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K46" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="L46" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="M46" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="N46" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="O46" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="P46" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="R46" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="S46" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="T46" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="U46" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="V46" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="W46" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="X46" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Y46" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="Z46" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="AA46" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AB46" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="8">
+        <v>500</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K47" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="L47" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="M47" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="N47" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="O47" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="P47" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="R47" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="S47" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="T47" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="U47" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="V47" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="W47" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="X47" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Y47" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="Z47" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="AA47" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AB47" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="8">
+        <v>1000</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K48" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="L48" s="1">
+        <v>2</v>
+      </c>
+      <c r="M48" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="N48" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="O48" s="1">
+        <v>2</v>
+      </c>
+      <c r="P48" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="R48" s="1">
+        <v>2</v>
+      </c>
+      <c r="S48" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="T48" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="U48" s="1">
+        <v>2</v>
+      </c>
+      <c r="V48" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="W48" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="X48" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y48" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="Z48" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="AA48" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB48" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="8">
+        <v>3000</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K49" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="L49" s="1">
+        <v>2</v>
+      </c>
+      <c r="M49" s="1">
+        <v>5</v>
+      </c>
+      <c r="N49" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="O49" s="1">
+        <v>2</v>
+      </c>
+      <c r="P49" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="R49" s="1">
+        <v>2</v>
+      </c>
+      <c r="S49" s="1">
+        <v>5</v>
+      </c>
+      <c r="T49" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="U49" s="1">
+        <v>2</v>
+      </c>
+      <c r="V49" s="1">
+        <v>5</v>
+      </c>
+      <c r="W49" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="X49" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y49" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z49" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="AA49" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB49" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="8">
+        <v>8000</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K50" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="L50" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="M50" s="1">
+        <v>4</v>
+      </c>
+      <c r="N50" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="O50" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="P50" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="R50" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="S50" s="1">
+        <v>4</v>
+      </c>
+      <c r="T50" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="U50" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="V50" s="1">
+        <v>4</v>
+      </c>
+      <c r="W50" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="X50" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="Y50" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z50" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="AA50" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AB50" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="8">
+        <v>100</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K51" s="7">
+        <v>23.669871794871799</v>
+      </c>
+      <c r="L51" s="1">
+        <v>14</v>
+      </c>
+      <c r="M51" s="1">
+        <v>30</v>
+      </c>
+      <c r="N51" s="7">
+        <v>23.669871794871799</v>
+      </c>
+      <c r="O51" s="1">
+        <v>14</v>
+      </c>
+      <c r="P51" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q51" s="7">
+        <v>23.669871794871799</v>
+      </c>
+      <c r="R51" s="1">
+        <v>14</v>
+      </c>
+      <c r="S51" s="1">
+        <v>30</v>
+      </c>
+      <c r="T51" s="7">
+        <v>23.669871794871799</v>
+      </c>
+      <c r="U51" s="1">
+        <v>14</v>
+      </c>
+      <c r="V51" s="1">
+        <v>30</v>
+      </c>
+      <c r="W51" s="7">
+        <v>23.669871794871799</v>
+      </c>
+      <c r="X51" s="1">
+        <v>14</v>
+      </c>
+      <c r="Y51" s="1">
+        <v>30</v>
+      </c>
+      <c r="Z51" s="7">
+        <v>23.669871794871799</v>
+      </c>
+      <c r="AA51" s="1">
+        <v>14</v>
+      </c>
+      <c r="AB51" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="8">
+        <v>500</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K52" s="7">
+        <v>23.669871794871799</v>
+      </c>
+      <c r="L52" s="1">
+        <v>14</v>
+      </c>
+      <c r="M52" s="1">
+        <v>30</v>
+      </c>
+      <c r="N52" s="7">
+        <v>23.669871794871799</v>
+      </c>
+      <c r="O52" s="1">
+        <v>14</v>
+      </c>
+      <c r="P52" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q52" s="7">
+        <v>23.669871794871799</v>
+      </c>
+      <c r="R52" s="1">
+        <v>14</v>
+      </c>
+      <c r="S52" s="1">
+        <v>30</v>
+      </c>
+      <c r="T52" s="7">
+        <v>23.669871794871799</v>
+      </c>
+      <c r="U52" s="1">
+        <v>14</v>
+      </c>
+      <c r="V52" s="1">
+        <v>30</v>
+      </c>
+      <c r="W52" s="7">
+        <v>23.669871794871799</v>
+      </c>
+      <c r="X52" s="1">
+        <v>14</v>
+      </c>
+      <c r="Y52" s="1">
+        <v>30</v>
+      </c>
+      <c r="Z52" s="7">
+        <v>23.669871794871799</v>
+      </c>
+      <c r="AA52" s="1">
+        <v>14</v>
+      </c>
+      <c r="AB52" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="8">
+        <v>1000</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K53" s="7">
+        <v>23.675000000000001</v>
+      </c>
+      <c r="L53" s="1">
+        <v>15</v>
+      </c>
+      <c r="M53" s="1">
+        <v>25</v>
+      </c>
+      <c r="N53" s="7">
+        <v>23.675000000000001</v>
+      </c>
+      <c r="O53" s="1">
+        <v>15</v>
+      </c>
+      <c r="P53" s="1">
+        <v>25</v>
+      </c>
+      <c r="Q53" s="7">
+        <v>23.675000000000001</v>
+      </c>
+      <c r="R53" s="1">
+        <v>15</v>
+      </c>
+      <c r="S53" s="1">
+        <v>25</v>
+      </c>
+      <c r="T53" s="7">
+        <v>23.675000000000001</v>
+      </c>
+      <c r="U53" s="1">
+        <v>15</v>
+      </c>
+      <c r="V53" s="1">
+        <v>25</v>
+      </c>
+      <c r="W53" s="7">
+        <v>23.675000000000001</v>
+      </c>
+      <c r="X53" s="1">
+        <v>15</v>
+      </c>
+      <c r="Y53" s="1">
+        <v>25</v>
+      </c>
+      <c r="Z53" s="7">
+        <v>23.675000000000001</v>
+      </c>
+      <c r="AA53" s="1">
+        <v>15</v>
+      </c>
+      <c r="AB53" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="8">
+        <v>3000</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K54" s="7">
+        <v>23.79</v>
+      </c>
+      <c r="L54" s="1">
+        <v>20</v>
+      </c>
+      <c r="M54" s="1">
+        <v>25</v>
+      </c>
+      <c r="N54" s="7">
+        <v>23.79</v>
+      </c>
+      <c r="O54" s="1">
+        <v>20</v>
+      </c>
+      <c r="P54" s="1">
+        <v>25</v>
+      </c>
+      <c r="Q54" s="7">
+        <v>23.79</v>
+      </c>
+      <c r="R54" s="1">
+        <v>20</v>
+      </c>
+      <c r="S54" s="1">
+        <v>25</v>
+      </c>
+      <c r="T54" s="7">
+        <v>23.79</v>
+      </c>
+      <c r="U54" s="1">
+        <v>20</v>
+      </c>
+      <c r="V54" s="1">
+        <v>25</v>
+      </c>
+      <c r="W54" s="7">
+        <v>23.79</v>
+      </c>
+      <c r="X54" s="1">
+        <v>20</v>
+      </c>
+      <c r="Y54" s="1">
+        <v>25</v>
+      </c>
+      <c r="Z54" s="7">
+        <v>23.79</v>
+      </c>
+      <c r="AA54" s="1">
+        <v>20</v>
+      </c>
+      <c r="AB54" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="8">
+        <v>8000</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K55" s="7">
+        <v>24.875</v>
+      </c>
+      <c r="L55" s="1">
+        <v>24</v>
+      </c>
+      <c r="M55" s="1">
+        <v>25</v>
+      </c>
+      <c r="N55" s="7">
+        <v>24.875</v>
+      </c>
+      <c r="O55" s="1">
+        <v>24</v>
+      </c>
+      <c r="P55" s="1">
+        <v>25</v>
+      </c>
+      <c r="Q55" s="7">
+        <v>24.875</v>
+      </c>
+      <c r="R55" s="1">
+        <v>24</v>
+      </c>
+      <c r="S55" s="1">
+        <v>25</v>
+      </c>
+      <c r="T55" s="7">
+        <v>24.875</v>
+      </c>
+      <c r="U55" s="1">
+        <v>24</v>
+      </c>
+      <c r="V55" s="1">
+        <v>25</v>
+      </c>
+      <c r="W55" s="7">
+        <v>24.875</v>
+      </c>
+      <c r="X55" s="1">
+        <v>24</v>
+      </c>
+      <c r="Y55" s="1">
+        <v>25</v>
+      </c>
+      <c r="Z55" s="7">
+        <v>24.875</v>
+      </c>
+      <c r="AA55" s="1">
+        <v>24</v>
+      </c>
+      <c r="AB55" s="1">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:Y43" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implement power curve code Calculate electricity production and load factor
</commit_message>
<xml_diff>
--- a/windisch/data/Input data.xlsx
+++ b/windisch/data/Input data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/windisch/windisch/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1350EE9-4A54-CD4C-A438-10D63DD0C550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085E71D5-EF78-0343-911D-196986A33A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5140" yWindow="760" windowWidth="23280" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="75">
   <si>
     <t>parameter</t>
   </si>
@@ -247,12 +247,6 @@
   </si>
   <si>
     <t>power</t>
-  </si>
-  <si>
-    <t>unitless</t>
-  </si>
-  <si>
-    <t>average capacity factor</t>
   </si>
   <si>
     <t>cut-in</t>
@@ -336,7 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -351,9 +345,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -667,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB55"/>
+  <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3693,76 +3684,82 @@
         <v>21</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>19</v>
+        <v>19</v>
+      </c>
+      <c r="C44" s="7">
+        <v>100</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="F44" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K44" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="L44" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="M44" s="6">
-        <v>0.45</v>
-      </c>
-      <c r="N44" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="O44" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="P44" s="6">
-        <v>0.45</v>
-      </c>
-      <c r="Q44" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="R44" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="S44" s="6">
-        <v>0.45</v>
-      </c>
-      <c r="T44" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="U44" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="V44" s="6">
-        <v>0.45</v>
-      </c>
-      <c r="W44" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="X44" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="Y44" s="6">
-        <v>0.45</v>
-      </c>
-      <c r="Z44" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="AA44" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="AB44" s="6">
-        <v>0.45</v>
+      <c r="K44" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="L44" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="M44" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="N44" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="O44" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="P44" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="R44" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="S44" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="T44" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="U44" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="V44" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="W44" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="X44" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Y44" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="Z44" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="AA44" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AB44" s="1">
+        <v>6.5</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.2">
@@ -3770,22 +3767,82 @@
         <v>21</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>19</v>
+        <v>19</v>
+      </c>
+      <c r="C45" s="7">
+        <v>500</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="F45" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>56</v>
+      </c>
+      <c r="K45" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="L45" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="M45" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="N45" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="O45" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="P45" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="R45" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="S45" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="T45" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="U45" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="V45" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="W45" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="X45" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Y45" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="Z45" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="AA45" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AB45" s="1">
+        <v>6.5</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.2">
@@ -3795,14 +3852,14 @@
       <c r="B46" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C46" s="8">
-        <v>100</v>
+      <c r="C46" s="7">
+        <v>1000</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>23</v>
@@ -3811,64 +3868,64 @@
         <v>18</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>56</v>
       </c>
       <c r="K46" s="1">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="L46" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="M46" s="1">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="N46" s="1">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="O46" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="P46" s="1">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="Q46" s="1">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="R46" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="S46" s="1">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="T46" s="1">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="U46" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V46" s="1">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="W46" s="1">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="X46" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="Y46" s="1">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="Z46" s="1">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="AA46" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB46" s="1">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.2">
@@ -3878,14 +3935,14 @@
       <c r="B47" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="8">
-        <v>500</v>
+      <c r="C47" s="7">
+        <v>3000</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>23</v>
@@ -3894,64 +3951,64 @@
         <v>18</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>56</v>
       </c>
       <c r="K47" s="1">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="L47" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="M47" s="1">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="N47" s="1">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="O47" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="P47" s="1">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="Q47" s="1">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="R47" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="S47" s="1">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="T47" s="1">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="U47" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V47" s="1">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="W47" s="1">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="X47" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="Y47" s="1">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="Z47" s="1">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="AA47" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB47" s="1">
-        <v>6.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.2">
@@ -3961,14 +4018,14 @@
       <c r="B48" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C48" s="8">
-        <v>1000</v>
+      <c r="C48" s="7">
+        <v>8000</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>23</v>
@@ -3977,64 +4034,64 @@
         <v>18</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>56</v>
       </c>
       <c r="K48" s="1">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="L48" s="1">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="M48" s="1">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="N48" s="1">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="O48" s="1">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="P48" s="1">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="Q48" s="1">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="R48" s="1">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="S48" s="1">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="T48" s="1">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="U48" s="1">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V48" s="1">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="W48" s="1">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="X48" s="1">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="Y48" s="1">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="Z48" s="1">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="AA48" s="1">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB48" s="1">
-        <v>5.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
@@ -4044,14 +4101,14 @@
       <c r="B49" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="8">
-        <v>3000</v>
+      <c r="C49" s="7">
+        <v>100</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>23</v>
@@ -4060,64 +4117,64 @@
         <v>18</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K49" s="1">
-        <v>3.1</v>
+      <c r="K49" s="6">
+        <v>23.669871794871799</v>
       </c>
       <c r="L49" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="M49" s="1">
-        <v>5</v>
-      </c>
-      <c r="N49" s="1">
-        <v>3.1</v>
+        <v>30</v>
+      </c>
+      <c r="N49" s="6">
+        <v>23.669871794871799</v>
       </c>
       <c r="O49" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="P49" s="1">
-        <v>5</v>
-      </c>
-      <c r="Q49" s="1">
-        <v>3.1</v>
+        <v>30</v>
+      </c>
+      <c r="Q49" s="6">
+        <v>23.669871794871799</v>
       </c>
       <c r="R49" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="S49" s="1">
-        <v>5</v>
-      </c>
-      <c r="T49" s="1">
-        <v>3.1</v>
+        <v>30</v>
+      </c>
+      <c r="T49" s="6">
+        <v>23.669871794871799</v>
       </c>
       <c r="U49" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="V49" s="1">
-        <v>5</v>
-      </c>
-      <c r="W49" s="1">
-        <v>3.1</v>
+        <v>30</v>
+      </c>
+      <c r="W49" s="6">
+        <v>23.669871794871799</v>
       </c>
       <c r="X49" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="Y49" s="1">
-        <v>5</v>
-      </c>
-      <c r="Z49" s="1">
-        <v>3.1</v>
+        <v>30</v>
+      </c>
+      <c r="Z49" s="6">
+        <v>23.669871794871799</v>
       </c>
       <c r="AA49" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="AB49" s="1">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.2">
@@ -4127,14 +4184,14 @@
       <c r="B50" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="8">
-        <v>8000</v>
+      <c r="C50" s="7">
+        <v>500</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>23</v>
@@ -4143,64 +4200,64 @@
         <v>18</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K50" s="1">
-        <v>3.1</v>
+      <c r="K50" s="6">
+        <v>23.669871794871799</v>
       </c>
       <c r="L50" s="1">
-        <v>2.5</v>
+        <v>14</v>
       </c>
       <c r="M50" s="1">
-        <v>4</v>
-      </c>
-      <c r="N50" s="1">
-        <v>3.1</v>
+        <v>30</v>
+      </c>
+      <c r="N50" s="6">
+        <v>23.669871794871799</v>
       </c>
       <c r="O50" s="1">
-        <v>2.5</v>
+        <v>14</v>
       </c>
       <c r="P50" s="1">
-        <v>4</v>
-      </c>
-      <c r="Q50" s="1">
-        <v>3.1</v>
+        <v>30</v>
+      </c>
+      <c r="Q50" s="6">
+        <v>23.669871794871799</v>
       </c>
       <c r="R50" s="1">
-        <v>2.5</v>
+        <v>14</v>
       </c>
       <c r="S50" s="1">
-        <v>4</v>
-      </c>
-      <c r="T50" s="1">
-        <v>3.1</v>
+        <v>30</v>
+      </c>
+      <c r="T50" s="6">
+        <v>23.669871794871799</v>
       </c>
       <c r="U50" s="1">
-        <v>2.5</v>
+        <v>14</v>
       </c>
       <c r="V50" s="1">
-        <v>4</v>
-      </c>
-      <c r="W50" s="1">
-        <v>3.1</v>
+        <v>30</v>
+      </c>
+      <c r="W50" s="6">
+        <v>23.669871794871799</v>
       </c>
       <c r="X50" s="1">
-        <v>2.5</v>
+        <v>14</v>
       </c>
       <c r="Y50" s="1">
-        <v>4</v>
-      </c>
-      <c r="Z50" s="1">
-        <v>3.1</v>
+        <v>30</v>
+      </c>
+      <c r="Z50" s="6">
+        <v>23.669871794871799</v>
       </c>
       <c r="AA50" s="1">
-        <v>2.5</v>
+        <v>14</v>
       </c>
       <c r="AB50" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.2">
@@ -4210,14 +4267,14 @@
       <c r="B51" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="8">
-        <v>100</v>
+      <c r="C51" s="7">
+        <v>1000</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>23</v>
@@ -4226,64 +4283,64 @@
         <v>18</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K51" s="7">
-        <v>23.669871794871799</v>
+      <c r="K51" s="6">
+        <v>23.675000000000001</v>
       </c>
       <c r="L51" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M51" s="1">
-        <v>30</v>
-      </c>
-      <c r="N51" s="7">
-        <v>23.669871794871799</v>
+        <v>25</v>
+      </c>
+      <c r="N51" s="6">
+        <v>23.675000000000001</v>
       </c>
       <c r="O51" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P51" s="1">
-        <v>30</v>
-      </c>
-      <c r="Q51" s="7">
-        <v>23.669871794871799</v>
+        <v>25</v>
+      </c>
+      <c r="Q51" s="6">
+        <v>23.675000000000001</v>
       </c>
       <c r="R51" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="S51" s="1">
-        <v>30</v>
-      </c>
-      <c r="T51" s="7">
-        <v>23.669871794871799</v>
+        <v>25</v>
+      </c>
+      <c r="T51" s="6">
+        <v>23.675000000000001</v>
       </c>
       <c r="U51" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="V51" s="1">
-        <v>30</v>
-      </c>
-      <c r="W51" s="7">
-        <v>23.669871794871799</v>
+        <v>25</v>
+      </c>
+      <c r="W51" s="6">
+        <v>23.675000000000001</v>
       </c>
       <c r="X51" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Y51" s="1">
-        <v>30</v>
-      </c>
-      <c r="Z51" s="7">
-        <v>23.669871794871799</v>
+        <v>25</v>
+      </c>
+      <c r="Z51" s="6">
+        <v>23.675000000000001</v>
       </c>
       <c r="AA51" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB51" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:28" x14ac:dyDescent="0.2">
@@ -4293,14 +4350,14 @@
       <c r="B52" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="8">
-        <v>500</v>
+      <c r="C52" s="7">
+        <v>3000</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>23</v>
@@ -4309,64 +4366,64 @@
         <v>18</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K52" s="7">
-        <v>23.669871794871799</v>
+      <c r="K52" s="6">
+        <v>23.79</v>
       </c>
       <c r="L52" s="1">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="M52" s="1">
-        <v>30</v>
-      </c>
-      <c r="N52" s="7">
-        <v>23.669871794871799</v>
+        <v>25</v>
+      </c>
+      <c r="N52" s="6">
+        <v>23.79</v>
       </c>
       <c r="O52" s="1">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="P52" s="1">
-        <v>30</v>
-      </c>
-      <c r="Q52" s="7">
-        <v>23.669871794871799</v>
+        <v>25</v>
+      </c>
+      <c r="Q52" s="6">
+        <v>23.79</v>
       </c>
       <c r="R52" s="1">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="S52" s="1">
-        <v>30</v>
-      </c>
-      <c r="T52" s="7">
-        <v>23.669871794871799</v>
+        <v>25</v>
+      </c>
+      <c r="T52" s="6">
+        <v>23.79</v>
       </c>
       <c r="U52" s="1">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="V52" s="1">
-        <v>30</v>
-      </c>
-      <c r="W52" s="7">
-        <v>23.669871794871799</v>
+        <v>25</v>
+      </c>
+      <c r="W52" s="6">
+        <v>23.79</v>
       </c>
       <c r="X52" s="1">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="Y52" s="1">
-        <v>30</v>
-      </c>
-      <c r="Z52" s="7">
-        <v>23.669871794871799</v>
+        <v>25</v>
+      </c>
+      <c r="Z52" s="6">
+        <v>23.79</v>
       </c>
       <c r="AA52" s="1">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="AB52" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.2">
@@ -4376,14 +4433,14 @@
       <c r="B53" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C53" s="8">
-        <v>1000</v>
+      <c r="C53" s="7">
+        <v>8000</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>23</v>
@@ -4392,229 +4449,63 @@
         <v>18</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K53" s="7">
-        <v>23.675000000000001</v>
+      <c r="K53" s="6">
+        <v>24.875</v>
       </c>
       <c r="L53" s="1">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="M53" s="1">
         <v>25</v>
       </c>
-      <c r="N53" s="7">
-        <v>23.675000000000001</v>
+      <c r="N53" s="6">
+        <v>24.875</v>
       </c>
       <c r="O53" s="1">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="P53" s="1">
         <v>25</v>
       </c>
-      <c r="Q53" s="7">
-        <v>23.675000000000001</v>
+      <c r="Q53" s="6">
+        <v>24.875</v>
       </c>
       <c r="R53" s="1">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="S53" s="1">
         <v>25</v>
       </c>
-      <c r="T53" s="7">
-        <v>23.675000000000001</v>
+      <c r="T53" s="6">
+        <v>24.875</v>
       </c>
       <c r="U53" s="1">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="V53" s="1">
         <v>25</v>
       </c>
-      <c r="W53" s="7">
-        <v>23.675000000000001</v>
+      <c r="W53" s="6">
+        <v>24.875</v>
       </c>
       <c r="X53" s="1">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="Y53" s="1">
         <v>25</v>
       </c>
-      <c r="Z53" s="7">
-        <v>23.675000000000001</v>
+      <c r="Z53" s="6">
+        <v>24.875</v>
       </c>
       <c r="AA53" s="1">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="AB53" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C54" s="8">
-        <v>3000</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K54" s="7">
-        <v>23.79</v>
-      </c>
-      <c r="L54" s="1">
-        <v>20</v>
-      </c>
-      <c r="M54" s="1">
-        <v>25</v>
-      </c>
-      <c r="N54" s="7">
-        <v>23.79</v>
-      </c>
-      <c r="O54" s="1">
-        <v>20</v>
-      </c>
-      <c r="P54" s="1">
-        <v>25</v>
-      </c>
-      <c r="Q54" s="7">
-        <v>23.79</v>
-      </c>
-      <c r="R54" s="1">
-        <v>20</v>
-      </c>
-      <c r="S54" s="1">
-        <v>25</v>
-      </c>
-      <c r="T54" s="7">
-        <v>23.79</v>
-      </c>
-      <c r="U54" s="1">
-        <v>20</v>
-      </c>
-      <c r="V54" s="1">
-        <v>25</v>
-      </c>
-      <c r="W54" s="7">
-        <v>23.79</v>
-      </c>
-      <c r="X54" s="1">
-        <v>20</v>
-      </c>
-      <c r="Y54" s="1">
-        <v>25</v>
-      </c>
-      <c r="Z54" s="7">
-        <v>23.79</v>
-      </c>
-      <c r="AA54" s="1">
-        <v>20</v>
-      </c>
-      <c r="AB54" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C55" s="8">
-        <v>8000</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K55" s="7">
-        <v>24.875</v>
-      </c>
-      <c r="L55" s="1">
-        <v>24</v>
-      </c>
-      <c r="M55" s="1">
-        <v>25</v>
-      </c>
-      <c r="N55" s="7">
-        <v>24.875</v>
-      </c>
-      <c r="O55" s="1">
-        <v>24</v>
-      </c>
-      <c r="P55" s="1">
-        <v>25</v>
-      </c>
-      <c r="Q55" s="7">
-        <v>24.875</v>
-      </c>
-      <c r="R55" s="1">
-        <v>24</v>
-      </c>
-      <c r="S55" s="1">
-        <v>25</v>
-      </c>
-      <c r="T55" s="7">
-        <v>24.875</v>
-      </c>
-      <c r="U55" s="1">
-        <v>24</v>
-      </c>
-      <c r="V55" s="1">
-        <v>25</v>
-      </c>
-      <c r="W55" s="7">
-        <v>24.875</v>
-      </c>
-      <c r="X55" s="1">
-        <v>24</v>
-      </c>
-      <c r="Y55" s="1">
-        <v>25</v>
-      </c>
-      <c r="Z55" s="7">
-        <v>24.875</v>
-      </c>
-      <c r="AA55" s="1">
-        <v>24</v>
-      </c>
-      <c r="AB55" s="1">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed distance from turbine to transformer, adn from transformer to coast
</commit_message>
<xml_diff>
--- a/windisch/data/Input data.xlsx
+++ b/windisch/data/Input data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/windisch/windisch/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085E71D5-EF78-0343-911D-196986A33A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE12815E-271A-754C-A281-39030B1197D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="760" windowWidth="23280" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35220" yWindow="40" windowWidth="23280" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$2:$Y$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$2:$Y$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -658,10 +658,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AC42" sqref="AC42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -845,7 +846,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -899,7 +900,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -953,7 +954,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1007,7 +1008,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1061,7 +1062,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1115,7 +1116,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -1290,7 +1291,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1385,7 +1386,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -1480,7 +1481,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1581,7 +1582,7 @@
         <v>10980</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1676,7 +1677,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1724,7 +1725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1772,7 +1773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1820,7 +1821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1868,7 +1869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1916,7 +1917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1964,7 +1965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -2012,7 +2013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -2060,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -2108,7 +2109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -2156,7 +2157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -2204,7 +2205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -2252,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -2300,7 +2301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
@@ -2395,7 +2396,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -2490,7 +2491,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
@@ -2591,7 +2592,7 @@
         <v>86.399999999999991</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>42</v>
       </c>
@@ -2686,7 +2687,7 @@
         <v>2592</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
@@ -2734,7 +2735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
@@ -2782,7 +2783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
@@ -2830,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
@@ -2878,7 +2879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
@@ -2973,7 +2974,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>47</v>
       </c>
@@ -3068,7 +3069,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>47</v>
       </c>
@@ -3163,7 +3164,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>21</v>
       </c>
@@ -3258,7 +3259,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>21</v>
       </c>
@@ -3353,7 +3354,7 @@
         <v>27.500000000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>24</v>
       </c>
@@ -3477,70 +3478,70 @@
         <v>56</v>
       </c>
       <c r="K41" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="L41" s="1">
         <f t="shared" si="27"/>
-        <v>45</v>
+        <v>0.9</v>
       </c>
       <c r="M41" s="1">
         <f t="shared" si="28"/>
-        <v>55.000000000000007</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N41" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="O41" s="1">
         <f t="shared" si="29"/>
-        <v>45</v>
+        <v>0.9</v>
       </c>
       <c r="P41" s="1">
         <f t="shared" si="30"/>
-        <v>55.000000000000007</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q41" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="R41" s="1">
         <f t="shared" si="31"/>
-        <v>45</v>
+        <v>0.9</v>
       </c>
       <c r="S41" s="1">
         <f t="shared" si="32"/>
-        <v>55.000000000000007</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="T41" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="U41" s="1">
         <f t="shared" si="33"/>
-        <v>45</v>
+        <v>0.9</v>
       </c>
       <c r="V41" s="1">
         <f t="shared" si="34"/>
-        <v>55.000000000000007</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="W41" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="X41" s="1">
         <f t="shared" si="35"/>
-        <v>45</v>
+        <v>0.9</v>
       </c>
       <c r="Y41" s="1">
         <f t="shared" si="36"/>
-        <v>55.000000000000007</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Z41" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="AA41" s="1">
         <f t="shared" si="37"/>
-        <v>45</v>
+        <v>0.9</v>
       </c>
       <c r="AB41" s="1">
         <f t="shared" si="38"/>
-        <v>55.000000000000007</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.2">
@@ -3572,73 +3573,73 @@
         <v>56</v>
       </c>
       <c r="K42" s="1">
-        <v>500</v>
+        <v>30</v>
       </c>
       <c r="L42" s="1">
         <f t="shared" si="27"/>
-        <v>450</v>
+        <v>27</v>
       </c>
       <c r="M42" s="1">
         <f t="shared" si="28"/>
-        <v>550</v>
+        <v>33</v>
       </c>
       <c r="N42" s="1">
-        <v>500</v>
+        <v>30</v>
       </c>
       <c r="O42" s="1">
         <f t="shared" si="29"/>
-        <v>450</v>
+        <v>27</v>
       </c>
       <c r="P42" s="1">
         <f t="shared" si="30"/>
-        <v>550</v>
+        <v>33</v>
       </c>
       <c r="Q42" s="1">
-        <v>500</v>
+        <v>30</v>
       </c>
       <c r="R42" s="1">
         <f t="shared" si="31"/>
-        <v>450</v>
+        <v>27</v>
       </c>
       <c r="S42" s="1">
         <f t="shared" si="32"/>
-        <v>550</v>
+        <v>33</v>
       </c>
       <c r="T42" s="1">
-        <v>500</v>
+        <v>30</v>
       </c>
       <c r="U42" s="1">
         <f t="shared" si="33"/>
-        <v>450</v>
+        <v>27</v>
       </c>
       <c r="V42" s="1">
         <f t="shared" si="34"/>
-        <v>550</v>
+        <v>33</v>
       </c>
       <c r="W42" s="1">
-        <v>500</v>
+        <v>30</v>
       </c>
       <c r="X42" s="1">
         <f t="shared" si="35"/>
-        <v>450</v>
+        <v>27</v>
       </c>
       <c r="Y42" s="1">
         <f t="shared" si="36"/>
-        <v>550</v>
+        <v>33</v>
       </c>
       <c r="Z42" s="1">
-        <v>500</v>
+        <v>30</v>
       </c>
       <c r="AA42" s="1">
         <f t="shared" si="37"/>
-        <v>450</v>
+        <v>27</v>
       </c>
       <c r="AB42" s="1">
         <f t="shared" si="38"/>
-        <v>550</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>24</v>
       </c>
@@ -3679,7 +3680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>21</v>
       </c>
@@ -3762,7 +3763,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>21</v>
       </c>
@@ -3845,7 +3846,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>21</v>
       </c>
@@ -3928,7 +3929,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>21</v>
       </c>
@@ -4011,7 +4012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>21</v>
       </c>
@@ -4094,7 +4095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>21</v>
       </c>
@@ -4177,7 +4178,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>21</v>
       </c>
@@ -4260,7 +4261,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>21</v>
       </c>
@@ -4343,7 +4344,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>21</v>
       </c>
@@ -4426,7 +4427,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>21</v>
       </c>
@@ -4510,7 +4511,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:Y43" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:Y53" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="distance to assembly plant"/>
+        <filter val="distance to coastline"/>
+        <filter val="distance to transformer"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>